<commit_message>
Before i start using Tuples
It is working here. About to start using tuples for the entire sheet and figuring out how to get the lists correct before going to find wattage
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/speedy/Documents/GitProjects/AmpSheetRepository/AmpSheetMain/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B02909-E921-6E45-97D7-1D4BF33717A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DA42B6-F7AF-9F4A-94EE-BBF0135AB3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20540" xr2:uid="{329AA3C5-52D5-8A41-A20D-B75AE869BCAA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20520" xr2:uid="{329AA3C5-52D5-8A41-A20D-B75AE869BCAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Racks" sheetId="1" r:id="rId1"/>
@@ -453,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -765,6 +765,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1100,10 +1101,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C41DDF0-49AF-A145-B81B-BCD86198E320}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AI104"/>
+  <dimension ref="A1:DU104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI4" sqref="AI4"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K93" sqref="K93:BS98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1112,7 +1113,7 @@
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="22">
+    <row r="1" spans="1:125" ht="22">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1140,7 +1141,7 @@
       <c r="I1" s="8"/>
       <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:35" ht="22">
+    <row r="2" spans="1:125" ht="22">
       <c r="A2" s="10"/>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -1164,7 +1165,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="22">
+    <row r="3" spans="1:125" ht="22">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1208,20 +1209,118 @@
       <c r="O3" s="92">
         <v>992</v>
       </c>
-      <c r="T3">
-        <v>1002</v>
-      </c>
-      <c r="Y3">
-        <v>1020</v>
-      </c>
-      <c r="Z3">
-        <v>1021</v>
-      </c>
-      <c r="AI3">
-        <v>1030</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" ht="22">
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="93"/>
+      <c r="S3" s="93"/>
+      <c r="T3" s="93"/>
+      <c r="U3" s="93"/>
+      <c r="V3" s="93"/>
+      <c r="W3" s="93"/>
+      <c r="X3" s="93"/>
+      <c r="Y3" s="93"/>
+      <c r="Z3" s="93"/>
+      <c r="AA3" s="93"/>
+      <c r="AB3" s="93"/>
+      <c r="AC3" s="93"/>
+      <c r="AD3" s="93"/>
+      <c r="AE3" s="93"/>
+      <c r="AF3" s="93"/>
+      <c r="AG3" s="93"/>
+      <c r="AH3" s="93"/>
+      <c r="AI3" s="93"/>
+      <c r="AJ3" s="93"/>
+      <c r="AK3" s="93"/>
+      <c r="AL3" s="93"/>
+      <c r="AM3" s="93"/>
+      <c r="AN3" s="93"/>
+      <c r="AO3" s="93"/>
+      <c r="AP3" s="93"/>
+      <c r="AQ3" s="93"/>
+      <c r="AR3" s="93"/>
+      <c r="AS3" s="93"/>
+      <c r="AT3" s="93"/>
+      <c r="AU3" s="93"/>
+      <c r="AV3" s="93"/>
+      <c r="AW3" s="93"/>
+      <c r="AX3" s="93"/>
+      <c r="AY3" s="93"/>
+      <c r="AZ3" s="93"/>
+      <c r="BA3" s="93"/>
+      <c r="BB3" s="93"/>
+      <c r="BC3" s="93"/>
+      <c r="BD3" s="93"/>
+      <c r="BE3" s="93"/>
+      <c r="BF3" s="93"/>
+      <c r="BG3" s="93"/>
+      <c r="BH3" s="93"/>
+      <c r="BI3" s="93"/>
+      <c r="BJ3" s="93"/>
+      <c r="BK3" s="93"/>
+      <c r="BL3" s="93"/>
+      <c r="BM3" s="93"/>
+      <c r="BN3" s="93"/>
+      <c r="BO3" s="93"/>
+      <c r="BP3" s="93"/>
+      <c r="BQ3" s="93"/>
+      <c r="BR3" s="93"/>
+      <c r="BS3" s="93"/>
+      <c r="BT3" s="93"/>
+      <c r="BU3" s="93"/>
+      <c r="BV3" s="93"/>
+      <c r="BW3" s="93"/>
+      <c r="BX3" s="93"/>
+      <c r="BY3" s="93"/>
+      <c r="BZ3" s="93"/>
+      <c r="CA3" s="93"/>
+      <c r="CB3" s="93"/>
+      <c r="CC3" s="93"/>
+      <c r="CD3" s="93"/>
+      <c r="CE3" s="93"/>
+      <c r="CF3" s="93"/>
+      <c r="CG3" s="93"/>
+      <c r="CH3" s="93"/>
+      <c r="CI3" s="93"/>
+      <c r="CJ3" s="93"/>
+      <c r="CK3" s="93"/>
+      <c r="CL3" s="93"/>
+      <c r="CM3" s="93"/>
+      <c r="CN3" s="93"/>
+      <c r="CO3" s="93"/>
+      <c r="CP3" s="93"/>
+      <c r="CQ3" s="93"/>
+      <c r="CR3" s="93"/>
+      <c r="CS3" s="93"/>
+      <c r="CT3" s="93"/>
+      <c r="CU3" s="93"/>
+      <c r="CV3" s="93"/>
+      <c r="CW3" s="93"/>
+      <c r="CX3" s="93"/>
+      <c r="CY3" s="93"/>
+      <c r="CZ3" s="93"/>
+      <c r="DA3" s="93"/>
+      <c r="DB3" s="93"/>
+      <c r="DC3" s="93"/>
+      <c r="DD3" s="93"/>
+      <c r="DE3" s="93"/>
+      <c r="DF3" s="93"/>
+      <c r="DG3" s="93"/>
+      <c r="DH3" s="93"/>
+      <c r="DI3" s="93"/>
+      <c r="DJ3" s="93"/>
+      <c r="DK3" s="93"/>
+      <c r="DL3" s="93"/>
+      <c r="DM3" s="93"/>
+      <c r="DN3" s="93"/>
+      <c r="DO3" s="93"/>
+      <c r="DP3" s="93"/>
+      <c r="DQ3" s="93"/>
+      <c r="DR3" s="93"/>
+      <c r="DS3" s="93"/>
+      <c r="DT3" s="93"/>
+      <c r="DU3" s="93"/>
+    </row>
+    <row r="4" spans="1:125" ht="22">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1250,8 +1349,123 @@
       <c r="J4" s="12">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:35" ht="22">
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="93"/>
+      <c r="P4" s="93"/>
+      <c r="Q4" s="93"/>
+      <c r="R4" s="93"/>
+      <c r="S4" s="93"/>
+      <c r="T4" s="93"/>
+      <c r="U4" s="93"/>
+      <c r="V4" s="93"/>
+      <c r="W4" s="93"/>
+      <c r="X4" s="93"/>
+      <c r="Y4" s="93"/>
+      <c r="Z4" s="93"/>
+      <c r="AA4" s="93"/>
+      <c r="AB4" s="93"/>
+      <c r="AC4" s="93"/>
+      <c r="AD4" s="93"/>
+      <c r="AE4" s="93"/>
+      <c r="AF4" s="93"/>
+      <c r="AG4" s="93"/>
+      <c r="AH4" s="93"/>
+      <c r="AI4" s="93"/>
+      <c r="AJ4" s="93"/>
+      <c r="AK4" s="93"/>
+      <c r="AL4" s="93"/>
+      <c r="AM4" s="93"/>
+      <c r="AN4" s="93"/>
+      <c r="AO4" s="93"/>
+      <c r="AP4" s="93"/>
+      <c r="AQ4" s="93"/>
+      <c r="AR4" s="93"/>
+      <c r="AS4" s="93"/>
+      <c r="AT4" s="93"/>
+      <c r="AU4" s="93"/>
+      <c r="AV4" s="93"/>
+      <c r="AW4" s="93"/>
+      <c r="AX4" s="93"/>
+      <c r="AY4" s="93"/>
+      <c r="AZ4" s="93"/>
+      <c r="BA4" s="93"/>
+      <c r="BB4" s="93"/>
+      <c r="BC4" s="93"/>
+      <c r="BD4" s="93"/>
+      <c r="BE4" s="93"/>
+      <c r="BF4" s="93"/>
+      <c r="BG4" s="93"/>
+      <c r="BH4" s="93"/>
+      <c r="BI4" s="93"/>
+      <c r="BJ4" s="93"/>
+      <c r="BK4" s="93"/>
+      <c r="BL4" s="93"/>
+      <c r="BM4" s="93"/>
+      <c r="BN4" s="93"/>
+      <c r="BO4" s="93"/>
+      <c r="BP4" s="93"/>
+      <c r="BQ4" s="93"/>
+      <c r="BR4" s="93"/>
+      <c r="BS4" s="93"/>
+      <c r="BT4" s="93"/>
+      <c r="BU4" s="93"/>
+      <c r="BV4" s="93"/>
+      <c r="BW4" s="93"/>
+      <c r="BX4" s="93"/>
+      <c r="BY4" s="93"/>
+      <c r="BZ4" s="93"/>
+      <c r="CA4" s="93"/>
+      <c r="CB4" s="93"/>
+      <c r="CC4" s="93"/>
+      <c r="CD4" s="93"/>
+      <c r="CE4" s="93"/>
+      <c r="CF4" s="93"/>
+      <c r="CG4" s="93"/>
+      <c r="CH4" s="93"/>
+      <c r="CI4" s="93"/>
+      <c r="CJ4" s="93"/>
+      <c r="CK4" s="93"/>
+      <c r="CL4" s="93"/>
+      <c r="CM4" s="93"/>
+      <c r="CN4" s="93"/>
+      <c r="CO4" s="93"/>
+      <c r="CP4" s="93"/>
+      <c r="CQ4" s="93"/>
+      <c r="CR4" s="93"/>
+      <c r="CS4" s="93"/>
+      <c r="CT4" s="93"/>
+      <c r="CU4" s="93"/>
+      <c r="CV4" s="93"/>
+      <c r="CW4" s="93"/>
+      <c r="CX4" s="93"/>
+      <c r="CY4" s="93"/>
+      <c r="CZ4" s="93"/>
+      <c r="DA4" s="93"/>
+      <c r="DB4" s="93"/>
+      <c r="DC4" s="93"/>
+      <c r="DD4" s="93"/>
+      <c r="DE4" s="93"/>
+      <c r="DF4" s="93"/>
+      <c r="DG4" s="93"/>
+      <c r="DH4" s="93"/>
+      <c r="DI4" s="93"/>
+      <c r="DJ4" s="93"/>
+      <c r="DK4" s="93"/>
+      <c r="DL4" s="93"/>
+      <c r="DM4" s="93"/>
+      <c r="DN4" s="93"/>
+      <c r="DO4" s="93"/>
+      <c r="DP4" s="93"/>
+      <c r="DQ4" s="93"/>
+      <c r="DR4" s="93"/>
+      <c r="DS4" s="93"/>
+      <c r="DT4" s="93"/>
+      <c r="DU4" s="93"/>
+    </row>
+    <row r="5" spans="1:125" ht="22">
       <c r="A5" s="4"/>
       <c r="B5" s="3">
         <v>3</v>
@@ -1272,8 +1486,123 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:35" ht="22">
+      <c r="K5" s="93"/>
+      <c r="L5" s="93"/>
+      <c r="M5" s="93"/>
+      <c r="N5" s="93"/>
+      <c r="O5" s="93"/>
+      <c r="P5" s="93"/>
+      <c r="Q5" s="93"/>
+      <c r="R5" s="93"/>
+      <c r="S5" s="93"/>
+      <c r="T5" s="93"/>
+      <c r="U5" s="93"/>
+      <c r="V5" s="93"/>
+      <c r="W5" s="93"/>
+      <c r="X5" s="93"/>
+      <c r="Y5" s="93"/>
+      <c r="Z5" s="93"/>
+      <c r="AA5" s="93"/>
+      <c r="AB5" s="93"/>
+      <c r="AC5" s="93"/>
+      <c r="AD5" s="93"/>
+      <c r="AE5" s="93"/>
+      <c r="AF5" s="93"/>
+      <c r="AG5" s="93"/>
+      <c r="AH5" s="93"/>
+      <c r="AI5" s="93"/>
+      <c r="AJ5" s="93"/>
+      <c r="AK5" s="93"/>
+      <c r="AL5" s="93"/>
+      <c r="AM5" s="93"/>
+      <c r="AN5" s="93"/>
+      <c r="AO5" s="93"/>
+      <c r="AP5" s="93"/>
+      <c r="AQ5" s="93"/>
+      <c r="AR5" s="93"/>
+      <c r="AS5" s="93"/>
+      <c r="AT5" s="93"/>
+      <c r="AU5" s="93"/>
+      <c r="AV5" s="93"/>
+      <c r="AW5" s="93"/>
+      <c r="AX5" s="93"/>
+      <c r="AY5" s="93"/>
+      <c r="AZ5" s="93"/>
+      <c r="BA5" s="93"/>
+      <c r="BB5" s="93"/>
+      <c r="BC5" s="93"/>
+      <c r="BD5" s="93"/>
+      <c r="BE5" s="93"/>
+      <c r="BF5" s="93"/>
+      <c r="BG5" s="93"/>
+      <c r="BH5" s="93"/>
+      <c r="BI5" s="93"/>
+      <c r="BJ5" s="93"/>
+      <c r="BK5" s="93"/>
+      <c r="BL5" s="93"/>
+      <c r="BM5" s="93"/>
+      <c r="BN5" s="93"/>
+      <c r="BO5" s="93"/>
+      <c r="BP5" s="93"/>
+      <c r="BQ5" s="93"/>
+      <c r="BR5" s="93"/>
+      <c r="BS5" s="93"/>
+      <c r="BT5" s="93"/>
+      <c r="BU5" s="93"/>
+      <c r="BV5" s="93"/>
+      <c r="BW5" s="93"/>
+      <c r="BX5" s="93"/>
+      <c r="BY5" s="93"/>
+      <c r="BZ5" s="93"/>
+      <c r="CA5" s="93"/>
+      <c r="CB5" s="93"/>
+      <c r="CC5" s="93"/>
+      <c r="CD5" s="93"/>
+      <c r="CE5" s="93"/>
+      <c r="CF5" s="93"/>
+      <c r="CG5" s="93"/>
+      <c r="CH5" s="93"/>
+      <c r="CI5" s="93"/>
+      <c r="CJ5" s="93"/>
+      <c r="CK5" s="93"/>
+      <c r="CL5" s="93"/>
+      <c r="CM5" s="93"/>
+      <c r="CN5" s="93"/>
+      <c r="CO5" s="93"/>
+      <c r="CP5" s="93"/>
+      <c r="CQ5" s="93"/>
+      <c r="CR5" s="93"/>
+      <c r="CS5" s="93"/>
+      <c r="CT5" s="93"/>
+      <c r="CU5" s="93"/>
+      <c r="CV5" s="93"/>
+      <c r="CW5" s="93"/>
+      <c r="CX5" s="93"/>
+      <c r="CY5" s="93"/>
+      <c r="CZ5" s="93"/>
+      <c r="DA5" s="93"/>
+      <c r="DB5" s="93"/>
+      <c r="DC5" s="93"/>
+      <c r="DD5" s="93"/>
+      <c r="DE5" s="93"/>
+      <c r="DF5" s="93"/>
+      <c r="DG5" s="93"/>
+      <c r="DH5" s="93"/>
+      <c r="DI5" s="93"/>
+      <c r="DJ5" s="93"/>
+      <c r="DK5" s="93"/>
+      <c r="DL5" s="93"/>
+      <c r="DM5" s="93"/>
+      <c r="DN5" s="93"/>
+      <c r="DO5" s="93"/>
+      <c r="DP5" s="93"/>
+      <c r="DQ5" s="93"/>
+      <c r="DR5" s="93"/>
+      <c r="DS5" s="93"/>
+      <c r="DT5" s="93"/>
+      <c r="DU5" s="93"/>
+    </row>
+    <row r="6" spans="1:125" ht="22">
       <c r="A6" s="4"/>
       <c r="B6" s="3">
         <v>4</v>
@@ -1300,8 +1629,123 @@
       <c r="J6" s="12">
         <v>907</v>
       </c>
-    </row>
-    <row r="7" spans="1:35" ht="22">
+      <c r="K6" s="93"/>
+      <c r="L6" s="93"/>
+      <c r="M6" s="93"/>
+      <c r="N6" s="93"/>
+      <c r="O6" s="93"/>
+      <c r="P6" s="93"/>
+      <c r="Q6" s="93"/>
+      <c r="R6" s="93"/>
+      <c r="S6" s="93"/>
+      <c r="T6" s="93"/>
+      <c r="U6" s="93"/>
+      <c r="V6" s="93"/>
+      <c r="W6" s="93"/>
+      <c r="X6" s="93"/>
+      <c r="Y6" s="93"/>
+      <c r="Z6" s="93"/>
+      <c r="AA6" s="93"/>
+      <c r="AB6" s="93"/>
+      <c r="AC6" s="93"/>
+      <c r="AD6" s="93"/>
+      <c r="AE6" s="93"/>
+      <c r="AF6" s="93"/>
+      <c r="AG6" s="93"/>
+      <c r="AH6" s="93"/>
+      <c r="AI6" s="93"/>
+      <c r="AJ6" s="93"/>
+      <c r="AK6" s="93"/>
+      <c r="AL6" s="93"/>
+      <c r="AM6" s="93"/>
+      <c r="AN6" s="93"/>
+      <c r="AO6" s="93"/>
+      <c r="AP6" s="93"/>
+      <c r="AQ6" s="93"/>
+      <c r="AR6" s="93"/>
+      <c r="AS6" s="93"/>
+      <c r="AT6" s="93"/>
+      <c r="AU6" s="93"/>
+      <c r="AV6" s="93"/>
+      <c r="AW6" s="93"/>
+      <c r="AX6" s="93"/>
+      <c r="AY6" s="93"/>
+      <c r="AZ6" s="93"/>
+      <c r="BA6" s="93"/>
+      <c r="BB6" s="93"/>
+      <c r="BC6" s="93"/>
+      <c r="BD6" s="93"/>
+      <c r="BE6" s="93"/>
+      <c r="BF6" s="93"/>
+      <c r="BG6" s="93"/>
+      <c r="BH6" s="93"/>
+      <c r="BI6" s="93"/>
+      <c r="BJ6" s="93"/>
+      <c r="BK6" s="93"/>
+      <c r="BL6" s="93"/>
+      <c r="BM6" s="93"/>
+      <c r="BN6" s="93"/>
+      <c r="BO6" s="93"/>
+      <c r="BP6" s="93"/>
+      <c r="BQ6" s="93"/>
+      <c r="BR6" s="93"/>
+      <c r="BS6" s="93"/>
+      <c r="BT6" s="93"/>
+      <c r="BU6" s="93"/>
+      <c r="BV6" s="93"/>
+      <c r="BW6" s="93"/>
+      <c r="BX6" s="93"/>
+      <c r="BY6" s="93"/>
+      <c r="BZ6" s="93"/>
+      <c r="CA6" s="93"/>
+      <c r="CB6" s="93"/>
+      <c r="CC6" s="93"/>
+      <c r="CD6" s="93"/>
+      <c r="CE6" s="93"/>
+      <c r="CF6" s="93"/>
+      <c r="CG6" s="93"/>
+      <c r="CH6" s="93"/>
+      <c r="CI6" s="93"/>
+      <c r="CJ6" s="93"/>
+      <c r="CK6" s="93"/>
+      <c r="CL6" s="93"/>
+      <c r="CM6" s="93"/>
+      <c r="CN6" s="93"/>
+      <c r="CO6" s="93"/>
+      <c r="CP6" s="93"/>
+      <c r="CQ6" s="93"/>
+      <c r="CR6" s="93"/>
+      <c r="CS6" s="93"/>
+      <c r="CT6" s="93"/>
+      <c r="CU6" s="93"/>
+      <c r="CV6" s="93"/>
+      <c r="CW6" s="93"/>
+      <c r="CX6" s="93"/>
+      <c r="CY6" s="93"/>
+      <c r="CZ6" s="93"/>
+      <c r="DA6" s="93"/>
+      <c r="DB6" s="93"/>
+      <c r="DC6" s="93"/>
+      <c r="DD6" s="93"/>
+      <c r="DE6" s="93"/>
+      <c r="DF6" s="93"/>
+      <c r="DG6" s="93"/>
+      <c r="DH6" s="93"/>
+      <c r="DI6" s="93"/>
+      <c r="DJ6" s="93"/>
+      <c r="DK6" s="93"/>
+      <c r="DL6" s="93"/>
+      <c r="DM6" s="93"/>
+      <c r="DN6" s="93"/>
+      <c r="DO6" s="93"/>
+      <c r="DP6" s="93"/>
+      <c r="DQ6" s="93"/>
+      <c r="DR6" s="93"/>
+      <c r="DS6" s="93"/>
+      <c r="DT6" s="93"/>
+      <c r="DU6" s="93"/>
+    </row>
+    <row r="7" spans="1:125" ht="22">
       <c r="A7" s="4"/>
       <c r="B7" s="3">
         <v>5</v>
@@ -1328,8 +1772,123 @@
       <c r="J7" s="12">
         <v>303</v>
       </c>
-    </row>
-    <row r="8" spans="1:35" ht="22">
+      <c r="K7" s="93"/>
+      <c r="L7" s="93"/>
+      <c r="M7" s="93"/>
+      <c r="N7" s="93"/>
+      <c r="O7" s="93"/>
+      <c r="P7" s="93"/>
+      <c r="Q7" s="93"/>
+      <c r="R7" s="93"/>
+      <c r="S7" s="93"/>
+      <c r="T7" s="93"/>
+      <c r="U7" s="93"/>
+      <c r="V7" s="93"/>
+      <c r="W7" s="93"/>
+      <c r="X7" s="93"/>
+      <c r="Y7" s="93"/>
+      <c r="Z7" s="93"/>
+      <c r="AA7" s="93"/>
+      <c r="AB7" s="93"/>
+      <c r="AC7" s="93"/>
+      <c r="AD7" s="93"/>
+      <c r="AE7" s="93"/>
+      <c r="AF7" s="93"/>
+      <c r="AG7" s="93"/>
+      <c r="AH7" s="93"/>
+      <c r="AI7" s="93"/>
+      <c r="AJ7" s="93"/>
+      <c r="AK7" s="93"/>
+      <c r="AL7" s="93"/>
+      <c r="AM7" s="93"/>
+      <c r="AN7" s="93"/>
+      <c r="AO7" s="93"/>
+      <c r="AP7" s="93"/>
+      <c r="AQ7" s="93"/>
+      <c r="AR7" s="93"/>
+      <c r="AS7" s="93"/>
+      <c r="AT7" s="93"/>
+      <c r="AU7" s="93"/>
+      <c r="AV7" s="93"/>
+      <c r="AW7" s="93"/>
+      <c r="AX7" s="93"/>
+      <c r="AY7" s="93"/>
+      <c r="AZ7" s="93"/>
+      <c r="BA7" s="93"/>
+      <c r="BB7" s="93"/>
+      <c r="BC7" s="93"/>
+      <c r="BD7" s="93"/>
+      <c r="BE7" s="93"/>
+      <c r="BF7" s="93"/>
+      <c r="BG7" s="93"/>
+      <c r="BH7" s="93"/>
+      <c r="BI7" s="93"/>
+      <c r="BJ7" s="93"/>
+      <c r="BK7" s="93"/>
+      <c r="BL7" s="93"/>
+      <c r="BM7" s="93"/>
+      <c r="BN7" s="93"/>
+      <c r="BO7" s="93"/>
+      <c r="BP7" s="93"/>
+      <c r="BQ7" s="93"/>
+      <c r="BR7" s="93"/>
+      <c r="BS7" s="93"/>
+      <c r="BT7" s="93"/>
+      <c r="BU7" s="93"/>
+      <c r="BV7" s="93"/>
+      <c r="BW7" s="93"/>
+      <c r="BX7" s="93"/>
+      <c r="BY7" s="93"/>
+      <c r="BZ7" s="93"/>
+      <c r="CA7" s="93"/>
+      <c r="CB7" s="93"/>
+      <c r="CC7" s="93"/>
+      <c r="CD7" s="93"/>
+      <c r="CE7" s="93"/>
+      <c r="CF7" s="93"/>
+      <c r="CG7" s="93"/>
+      <c r="CH7" s="93"/>
+      <c r="CI7" s="93"/>
+      <c r="CJ7" s="93"/>
+      <c r="CK7" s="93"/>
+      <c r="CL7" s="93"/>
+      <c r="CM7" s="93"/>
+      <c r="CN7" s="93"/>
+      <c r="CO7" s="93"/>
+      <c r="CP7" s="93"/>
+      <c r="CQ7" s="93"/>
+      <c r="CR7" s="93"/>
+      <c r="CS7" s="93"/>
+      <c r="CT7" s="93"/>
+      <c r="CU7" s="93"/>
+      <c r="CV7" s="93"/>
+      <c r="CW7" s="93"/>
+      <c r="CX7" s="93"/>
+      <c r="CY7" s="93"/>
+      <c r="CZ7" s="93"/>
+      <c r="DA7" s="93"/>
+      <c r="DB7" s="93"/>
+      <c r="DC7" s="93"/>
+      <c r="DD7" s="93"/>
+      <c r="DE7" s="93"/>
+      <c r="DF7" s="93"/>
+      <c r="DG7" s="93"/>
+      <c r="DH7" s="93"/>
+      <c r="DI7" s="93"/>
+      <c r="DJ7" s="93"/>
+      <c r="DK7" s="93"/>
+      <c r="DL7" s="93"/>
+      <c r="DM7" s="93"/>
+      <c r="DN7" s="93"/>
+      <c r="DO7" s="93"/>
+      <c r="DP7" s="93"/>
+      <c r="DQ7" s="93"/>
+      <c r="DR7" s="93"/>
+      <c r="DS7" s="93"/>
+      <c r="DT7" s="93"/>
+      <c r="DU7" s="93"/>
+    </row>
+    <row r="8" spans="1:125" ht="22">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -1350,8 +1909,123 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="12"/>
-    </row>
-    <row r="9" spans="1:35" ht="22">
+      <c r="K8" s="93"/>
+      <c r="L8" s="93"/>
+      <c r="M8" s="93"/>
+      <c r="N8" s="93"/>
+      <c r="O8" s="93"/>
+      <c r="P8" s="93"/>
+      <c r="Q8" s="93"/>
+      <c r="R8" s="93"/>
+      <c r="S8" s="93"/>
+      <c r="T8" s="93"/>
+      <c r="U8" s="93"/>
+      <c r="V8" s="93"/>
+      <c r="W8" s="93"/>
+      <c r="X8" s="93"/>
+      <c r="Y8" s="93"/>
+      <c r="Z8" s="93"/>
+      <c r="AA8" s="93"/>
+      <c r="AB8" s="93"/>
+      <c r="AC8" s="93"/>
+      <c r="AD8" s="93"/>
+      <c r="AE8" s="93"/>
+      <c r="AF8" s="93"/>
+      <c r="AG8" s="93"/>
+      <c r="AH8" s="93"/>
+      <c r="AI8" s="93"/>
+      <c r="AJ8" s="93"/>
+      <c r="AK8" s="93"/>
+      <c r="AL8" s="93"/>
+      <c r="AM8" s="93"/>
+      <c r="AN8" s="93"/>
+      <c r="AO8" s="93"/>
+      <c r="AP8" s="93"/>
+      <c r="AQ8" s="93"/>
+      <c r="AR8" s="93"/>
+      <c r="AS8" s="93"/>
+      <c r="AT8" s="93"/>
+      <c r="AU8" s="93"/>
+      <c r="AV8" s="93"/>
+      <c r="AW8" s="93"/>
+      <c r="AX8" s="93"/>
+      <c r="AY8" s="93"/>
+      <c r="AZ8" s="93"/>
+      <c r="BA8" s="93"/>
+      <c r="BB8" s="93"/>
+      <c r="BC8" s="93"/>
+      <c r="BD8" s="93"/>
+      <c r="BE8" s="93"/>
+      <c r="BF8" s="93"/>
+      <c r="BG8" s="93"/>
+      <c r="BH8" s="93"/>
+      <c r="BI8" s="93"/>
+      <c r="BJ8" s="93"/>
+      <c r="BK8" s="93"/>
+      <c r="BL8" s="93"/>
+      <c r="BM8" s="93"/>
+      <c r="BN8" s="93"/>
+      <c r="BO8" s="93"/>
+      <c r="BP8" s="93"/>
+      <c r="BQ8" s="93"/>
+      <c r="BR8" s="93"/>
+      <c r="BS8" s="93"/>
+      <c r="BT8" s="93"/>
+      <c r="BU8" s="93"/>
+      <c r="BV8" s="93"/>
+      <c r="BW8" s="93"/>
+      <c r="BX8" s="93"/>
+      <c r="BY8" s="93"/>
+      <c r="BZ8" s="93"/>
+      <c r="CA8" s="93"/>
+      <c r="CB8" s="93"/>
+      <c r="CC8" s="93"/>
+      <c r="CD8" s="93"/>
+      <c r="CE8" s="93"/>
+      <c r="CF8" s="93"/>
+      <c r="CG8" s="93"/>
+      <c r="CH8" s="93"/>
+      <c r="CI8" s="93"/>
+      <c r="CJ8" s="93"/>
+      <c r="CK8" s="93"/>
+      <c r="CL8" s="93"/>
+      <c r="CM8" s="93"/>
+      <c r="CN8" s="93"/>
+      <c r="CO8" s="93"/>
+      <c r="CP8" s="93"/>
+      <c r="CQ8" s="93"/>
+      <c r="CR8" s="93"/>
+      <c r="CS8" s="93"/>
+      <c r="CT8" s="93"/>
+      <c r="CU8" s="93"/>
+      <c r="CV8" s="93"/>
+      <c r="CW8" s="93"/>
+      <c r="CX8" s="93"/>
+      <c r="CY8" s="93"/>
+      <c r="CZ8" s="93"/>
+      <c r="DA8" s="93"/>
+      <c r="DB8" s="93"/>
+      <c r="DC8" s="93"/>
+      <c r="DD8" s="93"/>
+      <c r="DE8" s="93"/>
+      <c r="DF8" s="93"/>
+      <c r="DG8" s="93"/>
+      <c r="DH8" s="93"/>
+      <c r="DI8" s="93"/>
+      <c r="DJ8" s="93"/>
+      <c r="DK8" s="93"/>
+      <c r="DL8" s="93"/>
+      <c r="DM8" s="93"/>
+      <c r="DN8" s="93"/>
+      <c r="DO8" s="93"/>
+      <c r="DP8" s="93"/>
+      <c r="DQ8" s="93"/>
+      <c r="DR8" s="93"/>
+      <c r="DS8" s="93"/>
+      <c r="DT8" s="93"/>
+      <c r="DU8" s="93"/>
+    </row>
+    <row r="9" spans="1:125" ht="22">
       <c r="A9" s="61" t="s">
         <v>13</v>
       </c>
@@ -1380,7 +2054,7 @@
       <c r="I9" s="64"/>
       <c r="J9" s="65"/>
     </row>
-    <row r="10" spans="1:35" ht="24">
+    <row r="10" spans="1:125" ht="24">
       <c r="A10" s="62"/>
       <c r="B10" s="16" t="s">
         <v>26</v>
@@ -1400,7 +2074,7 @@
       <c r="I10" s="88"/>
       <c r="J10" s="89"/>
     </row>
-    <row r="11" spans="1:35" ht="22" customHeight="1">
+    <row r="11" spans="1:125" ht="22" customHeight="1">
       <c r="A11" s="74"/>
       <c r="B11" s="16"/>
       <c r="C11" s="50">
@@ -1418,7 +2092,7 @@
       <c r="I11" s="77"/>
       <c r="J11" s="78"/>
     </row>
-    <row r="12" spans="1:35" ht="22" customHeight="1">
+    <row r="12" spans="1:125" ht="22" customHeight="1">
       <c r="A12" s="75"/>
       <c r="B12" s="16"/>
       <c r="C12" s="53"/>
@@ -1430,7 +2104,7 @@
       <c r="I12" s="80"/>
       <c r="J12" s="81"/>
     </row>
-    <row r="13" spans="1:35" s="29" customFormat="1" ht="11">
+    <row r="13" spans="1:125" s="29" customFormat="1" ht="11">
       <c r="A13" s="56"/>
       <c r="B13" s="57"/>
       <c r="C13" s="57"/>
@@ -1442,7 +2116,7 @@
       <c r="I13" s="57"/>
       <c r="J13" s="58"/>
     </row>
-    <row r="14" spans="1:35" ht="22">
+    <row r="14" spans="1:125" ht="22">
       <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
@@ -1470,7 +2144,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:35" ht="22">
+    <row r="15" spans="1:125" ht="22">
       <c r="A15" s="17"/>
       <c r="B15" s="3" t="s">
         <v>8</v>
@@ -1494,7 +2168,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="22">
+    <row r="16" spans="1:125" ht="22">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -1517,8 +2191,59 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="1:10" ht="22">
+      <c r="K16" s="93">
+        <v>234</v>
+      </c>
+      <c r="L16" s="93">
+        <v>576</v>
+      </c>
+      <c r="M16" s="93"/>
+      <c r="N16" s="93"/>
+      <c r="O16" s="93"/>
+      <c r="P16" s="93"/>
+      <c r="Q16" s="93"/>
+      <c r="R16" s="93"/>
+      <c r="S16" s="93"/>
+      <c r="T16" s="93"/>
+      <c r="U16" s="93"/>
+      <c r="V16" s="93"/>
+      <c r="W16" s="93"/>
+      <c r="X16" s="93"/>
+      <c r="Y16" s="93"/>
+      <c r="Z16" s="93"/>
+      <c r="AA16" s="93"/>
+      <c r="AB16" s="93"/>
+      <c r="AC16" s="93"/>
+      <c r="AD16" s="93"/>
+      <c r="AE16" s="93"/>
+      <c r="AF16" s="93"/>
+      <c r="AG16" s="93"/>
+      <c r="AH16" s="93"/>
+      <c r="AI16" s="93"/>
+      <c r="AJ16" s="93"/>
+      <c r="AK16" s="93"/>
+      <c r="AL16" s="93"/>
+      <c r="AM16" s="93"/>
+      <c r="AN16" s="93"/>
+      <c r="AO16" s="93"/>
+      <c r="AP16" s="93"/>
+      <c r="AQ16" s="93"/>
+      <c r="AR16" s="93"/>
+      <c r="AS16" s="93"/>
+      <c r="AT16" s="93"/>
+      <c r="AU16" s="93"/>
+      <c r="AV16" s="93"/>
+      <c r="AW16" s="93"/>
+      <c r="AX16" s="93"/>
+      <c r="AY16" s="93"/>
+      <c r="AZ16" s="93"/>
+      <c r="BA16" s="93"/>
+      <c r="BB16" s="93"/>
+      <c r="BC16" s="93"/>
+      <c r="BD16" s="93"/>
+      <c r="BE16" s="93"/>
+    </row>
+    <row r="17" spans="1:121" ht="22">
       <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1539,8 +2264,55 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="12"/>
-    </row>
-    <row r="18" spans="1:10" ht="22">
+      <c r="K17" s="93"/>
+      <c r="L17" s="93"/>
+      <c r="M17" s="93"/>
+      <c r="N17" s="93"/>
+      <c r="O17" s="93"/>
+      <c r="P17" s="93"/>
+      <c r="Q17" s="93"/>
+      <c r="R17" s="93"/>
+      <c r="S17" s="93"/>
+      <c r="T17" s="93"/>
+      <c r="U17" s="93"/>
+      <c r="V17" s="93"/>
+      <c r="W17" s="93"/>
+      <c r="X17" s="93"/>
+      <c r="Y17" s="93"/>
+      <c r="Z17" s="93"/>
+      <c r="AA17" s="93"/>
+      <c r="AB17" s="93"/>
+      <c r="AC17" s="93"/>
+      <c r="AD17" s="93"/>
+      <c r="AE17" s="93"/>
+      <c r="AF17" s="93"/>
+      <c r="AG17" s="93"/>
+      <c r="AH17" s="93"/>
+      <c r="AI17" s="93"/>
+      <c r="AJ17" s="93"/>
+      <c r="AK17" s="93"/>
+      <c r="AL17" s="93"/>
+      <c r="AM17" s="93"/>
+      <c r="AN17" s="93"/>
+      <c r="AO17" s="93"/>
+      <c r="AP17" s="93"/>
+      <c r="AQ17" s="93"/>
+      <c r="AR17" s="93"/>
+      <c r="AS17" s="93"/>
+      <c r="AT17" s="93"/>
+      <c r="AU17" s="93"/>
+      <c r="AV17" s="93"/>
+      <c r="AW17" s="93"/>
+      <c r="AX17" s="93"/>
+      <c r="AY17" s="93"/>
+      <c r="AZ17" s="93"/>
+      <c r="BA17" s="93"/>
+      <c r="BB17" s="93"/>
+      <c r="BC17" s="93"/>
+      <c r="BD17" s="93"/>
+      <c r="BE17" s="93"/>
+    </row>
+    <row r="18" spans="1:121" ht="22">
       <c r="A18" s="4"/>
       <c r="B18" s="3">
         <v>3</v>
@@ -1565,8 +2337,55 @@
         <v>912</v>
       </c>
       <c r="J18" s="12"/>
-    </row>
-    <row r="19" spans="1:10" ht="22">
+      <c r="K18" s="93"/>
+      <c r="L18" s="93"/>
+      <c r="M18" s="93"/>
+      <c r="N18" s="93"/>
+      <c r="O18" s="93"/>
+      <c r="P18" s="93"/>
+      <c r="Q18" s="93"/>
+      <c r="R18" s="93"/>
+      <c r="S18" s="93"/>
+      <c r="T18" s="93"/>
+      <c r="U18" s="93"/>
+      <c r="V18" s="93"/>
+      <c r="W18" s="93"/>
+      <c r="X18" s="93"/>
+      <c r="Y18" s="93"/>
+      <c r="Z18" s="93"/>
+      <c r="AA18" s="93"/>
+      <c r="AB18" s="93"/>
+      <c r="AC18" s="93"/>
+      <c r="AD18" s="93"/>
+      <c r="AE18" s="93"/>
+      <c r="AF18" s="93"/>
+      <c r="AG18" s="93"/>
+      <c r="AH18" s="93"/>
+      <c r="AI18" s="93"/>
+      <c r="AJ18" s="93"/>
+      <c r="AK18" s="93"/>
+      <c r="AL18" s="93"/>
+      <c r="AM18" s="93"/>
+      <c r="AN18" s="93"/>
+      <c r="AO18" s="93"/>
+      <c r="AP18" s="93"/>
+      <c r="AQ18" s="93"/>
+      <c r="AR18" s="93"/>
+      <c r="AS18" s="93"/>
+      <c r="AT18" s="93"/>
+      <c r="AU18" s="93"/>
+      <c r="AV18" s="93"/>
+      <c r="AW18" s="93"/>
+      <c r="AX18" s="93"/>
+      <c r="AY18" s="93"/>
+      <c r="AZ18" s="93"/>
+      <c r="BA18" s="93"/>
+      <c r="BB18" s="93"/>
+      <c r="BC18" s="93"/>
+      <c r="BD18" s="93"/>
+      <c r="BE18" s="93"/>
+    </row>
+    <row r="19" spans="1:121" ht="22">
       <c r="A19" s="4"/>
       <c r="B19" s="3">
         <v>4</v>
@@ -1589,8 +2408,55 @@
         <v>6</v>
       </c>
       <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="1:10" ht="22">
+      <c r="K19" s="93"/>
+      <c r="L19" s="93"/>
+      <c r="M19" s="93"/>
+      <c r="N19" s="93"/>
+      <c r="O19" s="93"/>
+      <c r="P19" s="93"/>
+      <c r="Q19" s="93"/>
+      <c r="R19" s="93"/>
+      <c r="S19" s="93"/>
+      <c r="T19" s="93"/>
+      <c r="U19" s="93"/>
+      <c r="V19" s="93"/>
+      <c r="W19" s="93"/>
+      <c r="X19" s="93"/>
+      <c r="Y19" s="93"/>
+      <c r="Z19" s="93"/>
+      <c r="AA19" s="93"/>
+      <c r="AB19" s="93"/>
+      <c r="AC19" s="93"/>
+      <c r="AD19" s="93"/>
+      <c r="AE19" s="93"/>
+      <c r="AF19" s="93"/>
+      <c r="AG19" s="93"/>
+      <c r="AH19" s="93"/>
+      <c r="AI19" s="93"/>
+      <c r="AJ19" s="93"/>
+      <c r="AK19" s="93"/>
+      <c r="AL19" s="93"/>
+      <c r="AM19" s="93"/>
+      <c r="AN19" s="93"/>
+      <c r="AO19" s="93"/>
+      <c r="AP19" s="93"/>
+      <c r="AQ19" s="93"/>
+      <c r="AR19" s="93"/>
+      <c r="AS19" s="93"/>
+      <c r="AT19" s="93"/>
+      <c r="AU19" s="93"/>
+      <c r="AV19" s="93"/>
+      <c r="AW19" s="93"/>
+      <c r="AX19" s="93"/>
+      <c r="AY19" s="93"/>
+      <c r="AZ19" s="93"/>
+      <c r="BA19" s="93"/>
+      <c r="BB19" s="93"/>
+      <c r="BC19" s="93"/>
+      <c r="BD19" s="93"/>
+      <c r="BE19" s="93"/>
+    </row>
+    <row r="20" spans="1:121" ht="22">
       <c r="A20" s="4"/>
       <c r="B20" s="3">
         <v>5</v>
@@ -1617,8 +2483,55 @@
       <c r="J20" s="12">
         <v>309</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="22">
+      <c r="K20" s="93"/>
+      <c r="L20" s="93"/>
+      <c r="M20" s="93"/>
+      <c r="N20" s="93"/>
+      <c r="O20" s="93"/>
+      <c r="P20" s="93"/>
+      <c r="Q20" s="93"/>
+      <c r="R20" s="93"/>
+      <c r="S20" s="93"/>
+      <c r="T20" s="93"/>
+      <c r="U20" s="93"/>
+      <c r="V20" s="93"/>
+      <c r="W20" s="93"/>
+      <c r="X20" s="93"/>
+      <c r="Y20" s="93"/>
+      <c r="Z20" s="93"/>
+      <c r="AA20" s="93"/>
+      <c r="AB20" s="93"/>
+      <c r="AC20" s="93"/>
+      <c r="AD20" s="93"/>
+      <c r="AE20" s="93"/>
+      <c r="AF20" s="93"/>
+      <c r="AG20" s="93"/>
+      <c r="AH20" s="93"/>
+      <c r="AI20" s="93"/>
+      <c r="AJ20" s="93"/>
+      <c r="AK20" s="93"/>
+      <c r="AL20" s="93"/>
+      <c r="AM20" s="93"/>
+      <c r="AN20" s="93"/>
+      <c r="AO20" s="93"/>
+      <c r="AP20" s="93"/>
+      <c r="AQ20" s="93"/>
+      <c r="AR20" s="93"/>
+      <c r="AS20" s="93"/>
+      <c r="AT20" s="93"/>
+      <c r="AU20" s="93"/>
+      <c r="AV20" s="93"/>
+      <c r="AW20" s="93"/>
+      <c r="AX20" s="93"/>
+      <c r="AY20" s="93"/>
+      <c r="AZ20" s="93"/>
+      <c r="BA20" s="93"/>
+      <c r="BB20" s="93"/>
+      <c r="BC20" s="93"/>
+      <c r="BD20" s="93"/>
+      <c r="BE20" s="93"/>
+    </row>
+    <row r="21" spans="1:121" ht="22">
       <c r="A21" s="3" t="s">
         <v>12</v>
       </c>
@@ -1639,8 +2552,55 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="12"/>
-    </row>
-    <row r="22" spans="1:10" ht="22">
+      <c r="K21" s="93"/>
+      <c r="L21" s="93"/>
+      <c r="M21" s="93"/>
+      <c r="N21" s="93"/>
+      <c r="O21" s="93"/>
+      <c r="P21" s="93"/>
+      <c r="Q21" s="93"/>
+      <c r="R21" s="93"/>
+      <c r="S21" s="93"/>
+      <c r="T21" s="93"/>
+      <c r="U21" s="93"/>
+      <c r="V21" s="93"/>
+      <c r="W21" s="93"/>
+      <c r="X21" s="93"/>
+      <c r="Y21" s="93"/>
+      <c r="Z21" s="93"/>
+      <c r="AA21" s="93"/>
+      <c r="AB21" s="93"/>
+      <c r="AC21" s="93"/>
+      <c r="AD21" s="93"/>
+      <c r="AE21" s="93"/>
+      <c r="AF21" s="93"/>
+      <c r="AG21" s="93"/>
+      <c r="AH21" s="93"/>
+      <c r="AI21" s="93"/>
+      <c r="AJ21" s="93"/>
+      <c r="AK21" s="93"/>
+      <c r="AL21" s="93"/>
+      <c r="AM21" s="93"/>
+      <c r="AN21" s="93"/>
+      <c r="AO21" s="93"/>
+      <c r="AP21" s="93"/>
+      <c r="AQ21" s="93"/>
+      <c r="AR21" s="93"/>
+      <c r="AS21" s="93"/>
+      <c r="AT21" s="93"/>
+      <c r="AU21" s="93"/>
+      <c r="AV21" s="93"/>
+      <c r="AW21" s="93"/>
+      <c r="AX21" s="93"/>
+      <c r="AY21" s="93"/>
+      <c r="AZ21" s="93"/>
+      <c r="BA21" s="93"/>
+      <c r="BB21" s="93"/>
+      <c r="BC21" s="93"/>
+      <c r="BD21" s="93"/>
+      <c r="BE21" s="93"/>
+    </row>
+    <row r="22" spans="1:121" ht="22">
       <c r="A22" s="61" t="s">
         <v>16</v>
       </c>
@@ -1669,7 +2629,7 @@
       <c r="I22" s="64"/>
       <c r="J22" s="65"/>
     </row>
-    <row r="23" spans="1:10" ht="22">
+    <row r="23" spans="1:121" ht="22">
       <c r="A23" s="62"/>
       <c r="B23" s="16" t="s">
         <v>26</v>
@@ -1689,7 +2649,7 @@
       <c r="I23" s="64"/>
       <c r="J23" s="65"/>
     </row>
-    <row r="24" spans="1:10" ht="22" customHeight="1">
+    <row r="24" spans="1:121" ht="22" customHeight="1">
       <c r="A24" s="68"/>
       <c r="B24" s="66" t="s">
         <v>28</v>
@@ -1709,7 +2669,7 @@
       <c r="I24" s="42"/>
       <c r="J24" s="43"/>
     </row>
-    <row r="25" spans="1:10" ht="22" customHeight="1">
+    <row r="25" spans="1:121" ht="22" customHeight="1">
       <c r="A25" s="69"/>
       <c r="B25" s="67"/>
       <c r="C25" s="44"/>
@@ -1721,7 +2681,7 @@
       <c r="I25" s="45"/>
       <c r="J25" s="46"/>
     </row>
-    <row r="26" spans="1:10" ht="22">
+    <row r="26" spans="1:121" ht="22">
       <c r="A26" s="3" t="s">
         <v>3</v>
       </c>
@@ -1749,7 +2709,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="9"/>
     </row>
-    <row r="27" spans="1:10" ht="22">
+    <row r="27" spans="1:121" ht="22">
       <c r="A27" s="10"/>
       <c r="B27" s="3" t="s">
         <v>8</v>
@@ -1773,7 +2733,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="22">
+    <row r="28" spans="1:121" ht="22">
       <c r="A28" s="3" t="s">
         <v>10</v>
       </c>
@@ -1796,8 +2756,119 @@
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="12"/>
-    </row>
-    <row r="29" spans="1:10" ht="22">
+      <c r="K28" s="93"/>
+      <c r="L28" s="93"/>
+      <c r="M28" s="93"/>
+      <c r="N28" s="93"/>
+      <c r="O28" s="93"/>
+      <c r="P28" s="93"/>
+      <c r="Q28" s="93"/>
+      <c r="R28" s="93"/>
+      <c r="S28" s="93"/>
+      <c r="T28" s="93"/>
+      <c r="U28" s="93"/>
+      <c r="V28" s="93"/>
+      <c r="W28" s="93"/>
+      <c r="X28" s="93"/>
+      <c r="Y28" s="93"/>
+      <c r="Z28" s="93"/>
+      <c r="AA28" s="93"/>
+      <c r="AB28" s="93"/>
+      <c r="AC28" s="93"/>
+      <c r="AD28" s="93"/>
+      <c r="AE28" s="93"/>
+      <c r="AF28" s="93"/>
+      <c r="AG28" s="93"/>
+      <c r="AH28" s="93"/>
+      <c r="AI28" s="93"/>
+      <c r="AJ28" s="93"/>
+      <c r="AK28" s="93"/>
+      <c r="AL28" s="93"/>
+      <c r="AM28" s="93"/>
+      <c r="AN28" s="93"/>
+      <c r="AO28" s="93"/>
+      <c r="AP28" s="93"/>
+      <c r="AQ28" s="93"/>
+      <c r="AR28" s="93"/>
+      <c r="AS28" s="93"/>
+      <c r="AT28" s="93"/>
+      <c r="AU28" s="93"/>
+      <c r="AV28" s="93"/>
+      <c r="AW28" s="93"/>
+      <c r="AX28" s="93"/>
+      <c r="AY28" s="93"/>
+      <c r="AZ28" s="93"/>
+      <c r="BA28" s="93"/>
+      <c r="BB28" s="93"/>
+      <c r="BC28" s="93"/>
+      <c r="BD28" s="93"/>
+      <c r="BE28" s="93"/>
+      <c r="BF28" s="93"/>
+      <c r="BG28" s="93"/>
+      <c r="BH28" s="93"/>
+      <c r="BI28" s="93"/>
+      <c r="BJ28" s="93"/>
+      <c r="BK28" s="93"/>
+      <c r="BL28" s="93"/>
+      <c r="BM28" s="93"/>
+      <c r="BN28" s="93"/>
+      <c r="BO28" s="93"/>
+      <c r="BP28" s="93"/>
+      <c r="BQ28" s="93"/>
+      <c r="BR28" s="93"/>
+      <c r="BS28" s="93"/>
+      <c r="BT28" s="93"/>
+      <c r="BU28" s="93"/>
+      <c r="BV28" s="93"/>
+      <c r="BW28" s="93"/>
+      <c r="BX28" s="93"/>
+      <c r="BY28" s="93"/>
+      <c r="BZ28" s="93"/>
+      <c r="CA28" s="93"/>
+      <c r="CB28" s="93"/>
+      <c r="CC28" s="93"/>
+      <c r="CD28" s="93"/>
+      <c r="CE28" s="93"/>
+      <c r="CF28" s="93"/>
+      <c r="CG28" s="93"/>
+      <c r="CH28" s="93"/>
+      <c r="CI28" s="93"/>
+      <c r="CJ28" s="93"/>
+      <c r="CK28" s="93"/>
+      <c r="CL28" s="93"/>
+      <c r="CM28" s="93"/>
+      <c r="CN28" s="93"/>
+      <c r="CO28" s="93"/>
+      <c r="CP28" s="93"/>
+      <c r="CQ28" s="93"/>
+      <c r="CR28" s="93"/>
+      <c r="CS28" s="93"/>
+      <c r="CT28" s="93"/>
+      <c r="CU28" s="93"/>
+      <c r="CV28" s="93"/>
+      <c r="CW28" s="93"/>
+      <c r="CX28" s="93"/>
+      <c r="CY28" s="93"/>
+      <c r="CZ28" s="93"/>
+      <c r="DA28" s="93"/>
+      <c r="DB28" s="93"/>
+      <c r="DC28" s="93"/>
+      <c r="DD28" s="93"/>
+      <c r="DE28" s="93"/>
+      <c r="DF28" s="93"/>
+      <c r="DG28" s="93"/>
+      <c r="DH28" s="93"/>
+      <c r="DI28" s="93"/>
+      <c r="DJ28" s="93"/>
+      <c r="DK28" s="93"/>
+      <c r="DL28" s="93"/>
+      <c r="DM28" s="93"/>
+      <c r="DN28" s="93"/>
+      <c r="DO28" s="93"/>
+      <c r="DP28" s="93"/>
+      <c r="DQ28" s="93"/>
+    </row>
+    <row r="29" spans="1:121" ht="22">
       <c r="A29" s="3" t="s">
         <v>11</v>
       </c>
@@ -1826,8 +2897,119 @@
       <c r="J29" s="12">
         <v>916</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="22">
+      <c r="K29" s="93"/>
+      <c r="L29" s="93"/>
+      <c r="M29" s="93"/>
+      <c r="N29" s="93"/>
+      <c r="O29" s="93"/>
+      <c r="P29" s="93"/>
+      <c r="Q29" s="93"/>
+      <c r="R29" s="93"/>
+      <c r="S29" s="93"/>
+      <c r="T29" s="93"/>
+      <c r="U29" s="93"/>
+      <c r="V29" s="93"/>
+      <c r="W29" s="93"/>
+      <c r="X29" s="93"/>
+      <c r="Y29" s="93"/>
+      <c r="Z29" s="93"/>
+      <c r="AA29" s="93"/>
+      <c r="AB29" s="93"/>
+      <c r="AC29" s="93"/>
+      <c r="AD29" s="93"/>
+      <c r="AE29" s="93"/>
+      <c r="AF29" s="93"/>
+      <c r="AG29" s="93"/>
+      <c r="AH29" s="93"/>
+      <c r="AI29" s="93"/>
+      <c r="AJ29" s="93"/>
+      <c r="AK29" s="93"/>
+      <c r="AL29" s="93"/>
+      <c r="AM29" s="93"/>
+      <c r="AN29" s="93"/>
+      <c r="AO29" s="93"/>
+      <c r="AP29" s="93"/>
+      <c r="AQ29" s="93"/>
+      <c r="AR29" s="93"/>
+      <c r="AS29" s="93"/>
+      <c r="AT29" s="93"/>
+      <c r="AU29" s="93"/>
+      <c r="AV29" s="93"/>
+      <c r="AW29" s="93"/>
+      <c r="AX29" s="93"/>
+      <c r="AY29" s="93"/>
+      <c r="AZ29" s="93"/>
+      <c r="BA29" s="93"/>
+      <c r="BB29" s="93"/>
+      <c r="BC29" s="93"/>
+      <c r="BD29" s="93"/>
+      <c r="BE29" s="93"/>
+      <c r="BF29" s="93"/>
+      <c r="BG29" s="93"/>
+      <c r="BH29" s="93"/>
+      <c r="BI29" s="93"/>
+      <c r="BJ29" s="93"/>
+      <c r="BK29" s="93"/>
+      <c r="BL29" s="93"/>
+      <c r="BM29" s="93"/>
+      <c r="BN29" s="93"/>
+      <c r="BO29" s="93"/>
+      <c r="BP29" s="93"/>
+      <c r="BQ29" s="93"/>
+      <c r="BR29" s="93"/>
+      <c r="BS29" s="93"/>
+      <c r="BT29" s="93"/>
+      <c r="BU29" s="93"/>
+      <c r="BV29" s="93"/>
+      <c r="BW29" s="93"/>
+      <c r="BX29" s="93"/>
+      <c r="BY29" s="93"/>
+      <c r="BZ29" s="93"/>
+      <c r="CA29" s="93"/>
+      <c r="CB29" s="93"/>
+      <c r="CC29" s="93"/>
+      <c r="CD29" s="93"/>
+      <c r="CE29" s="93"/>
+      <c r="CF29" s="93"/>
+      <c r="CG29" s="93"/>
+      <c r="CH29" s="93"/>
+      <c r="CI29" s="93"/>
+      <c r="CJ29" s="93"/>
+      <c r="CK29" s="93"/>
+      <c r="CL29" s="93"/>
+      <c r="CM29" s="93"/>
+      <c r="CN29" s="93"/>
+      <c r="CO29" s="93"/>
+      <c r="CP29" s="93"/>
+      <c r="CQ29" s="93"/>
+      <c r="CR29" s="93"/>
+      <c r="CS29" s="93"/>
+      <c r="CT29" s="93"/>
+      <c r="CU29" s="93"/>
+      <c r="CV29" s="93"/>
+      <c r="CW29" s="93"/>
+      <c r="CX29" s="93"/>
+      <c r="CY29" s="93"/>
+      <c r="CZ29" s="93"/>
+      <c r="DA29" s="93"/>
+      <c r="DB29" s="93"/>
+      <c r="DC29" s="93"/>
+      <c r="DD29" s="93"/>
+      <c r="DE29" s="93"/>
+      <c r="DF29" s="93"/>
+      <c r="DG29" s="93"/>
+      <c r="DH29" s="93"/>
+      <c r="DI29" s="93"/>
+      <c r="DJ29" s="93"/>
+      <c r="DK29" s="93"/>
+      <c r="DL29" s="93"/>
+      <c r="DM29" s="93"/>
+      <c r="DN29" s="93"/>
+      <c r="DO29" s="93"/>
+      <c r="DP29" s="93"/>
+      <c r="DQ29" s="93"/>
+    </row>
+    <row r="30" spans="1:121" ht="22">
       <c r="A30" s="4"/>
       <c r="B30" s="3">
         <v>3</v>
@@ -1850,8 +3032,119 @@
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="12"/>
-    </row>
-    <row r="31" spans="1:10" ht="22">
+      <c r="K30" s="93"/>
+      <c r="L30" s="93"/>
+      <c r="M30" s="93"/>
+      <c r="N30" s="93"/>
+      <c r="O30" s="93"/>
+      <c r="P30" s="93"/>
+      <c r="Q30" s="93"/>
+      <c r="R30" s="93"/>
+      <c r="S30" s="93"/>
+      <c r="T30" s="93"/>
+      <c r="U30" s="93"/>
+      <c r="V30" s="93"/>
+      <c r="W30" s="93"/>
+      <c r="X30" s="93"/>
+      <c r="Y30" s="93"/>
+      <c r="Z30" s="93"/>
+      <c r="AA30" s="93"/>
+      <c r="AB30" s="93"/>
+      <c r="AC30" s="93"/>
+      <c r="AD30" s="93"/>
+      <c r="AE30" s="93"/>
+      <c r="AF30" s="93"/>
+      <c r="AG30" s="93"/>
+      <c r="AH30" s="93"/>
+      <c r="AI30" s="93"/>
+      <c r="AJ30" s="93"/>
+      <c r="AK30" s="93"/>
+      <c r="AL30" s="93"/>
+      <c r="AM30" s="93"/>
+      <c r="AN30" s="93"/>
+      <c r="AO30" s="93"/>
+      <c r="AP30" s="93"/>
+      <c r="AQ30" s="93"/>
+      <c r="AR30" s="93"/>
+      <c r="AS30" s="93"/>
+      <c r="AT30" s="93"/>
+      <c r="AU30" s="93"/>
+      <c r="AV30" s="93"/>
+      <c r="AW30" s="93"/>
+      <c r="AX30" s="93"/>
+      <c r="AY30" s="93"/>
+      <c r="AZ30" s="93"/>
+      <c r="BA30" s="93"/>
+      <c r="BB30" s="93"/>
+      <c r="BC30" s="93"/>
+      <c r="BD30" s="93"/>
+      <c r="BE30" s="93"/>
+      <c r="BF30" s="93"/>
+      <c r="BG30" s="93"/>
+      <c r="BH30" s="93"/>
+      <c r="BI30" s="93"/>
+      <c r="BJ30" s="93"/>
+      <c r="BK30" s="93"/>
+      <c r="BL30" s="93"/>
+      <c r="BM30" s="93"/>
+      <c r="BN30" s="93"/>
+      <c r="BO30" s="93"/>
+      <c r="BP30" s="93"/>
+      <c r="BQ30" s="93"/>
+      <c r="BR30" s="93"/>
+      <c r="BS30" s="93"/>
+      <c r="BT30" s="93"/>
+      <c r="BU30" s="93"/>
+      <c r="BV30" s="93"/>
+      <c r="BW30" s="93"/>
+      <c r="BX30" s="93"/>
+      <c r="BY30" s="93"/>
+      <c r="BZ30" s="93"/>
+      <c r="CA30" s="93"/>
+      <c r="CB30" s="93"/>
+      <c r="CC30" s="93"/>
+      <c r="CD30" s="93"/>
+      <c r="CE30" s="93"/>
+      <c r="CF30" s="93"/>
+      <c r="CG30" s="93"/>
+      <c r="CH30" s="93"/>
+      <c r="CI30" s="93"/>
+      <c r="CJ30" s="93"/>
+      <c r="CK30" s="93"/>
+      <c r="CL30" s="93"/>
+      <c r="CM30" s="93"/>
+      <c r="CN30" s="93"/>
+      <c r="CO30" s="93"/>
+      <c r="CP30" s="93"/>
+      <c r="CQ30" s="93"/>
+      <c r="CR30" s="93"/>
+      <c r="CS30" s="93"/>
+      <c r="CT30" s="93"/>
+      <c r="CU30" s="93"/>
+      <c r="CV30" s="93"/>
+      <c r="CW30" s="93"/>
+      <c r="CX30" s="93"/>
+      <c r="CY30" s="93"/>
+      <c r="CZ30" s="93"/>
+      <c r="DA30" s="93"/>
+      <c r="DB30" s="93"/>
+      <c r="DC30" s="93"/>
+      <c r="DD30" s="93"/>
+      <c r="DE30" s="93"/>
+      <c r="DF30" s="93"/>
+      <c r="DG30" s="93"/>
+      <c r="DH30" s="93"/>
+      <c r="DI30" s="93"/>
+      <c r="DJ30" s="93"/>
+      <c r="DK30" s="93"/>
+      <c r="DL30" s="93"/>
+      <c r="DM30" s="93"/>
+      <c r="DN30" s="93"/>
+      <c r="DO30" s="93"/>
+      <c r="DP30" s="93"/>
+      <c r="DQ30" s="93"/>
+    </row>
+    <row r="31" spans="1:121" ht="22">
       <c r="A31" s="4"/>
       <c r="B31" s="3">
         <v>4</v>
@@ -1878,8 +3171,119 @@
       <c r="J31" s="12">
         <v>313</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="22">
+      <c r="K31" s="93"/>
+      <c r="L31" s="93"/>
+      <c r="M31" s="93"/>
+      <c r="N31" s="93"/>
+      <c r="O31" s="93"/>
+      <c r="P31" s="93"/>
+      <c r="Q31" s="93"/>
+      <c r="R31" s="93"/>
+      <c r="S31" s="93"/>
+      <c r="T31" s="93"/>
+      <c r="U31" s="93"/>
+      <c r="V31" s="93"/>
+      <c r="W31" s="93"/>
+      <c r="X31" s="93"/>
+      <c r="Y31" s="93"/>
+      <c r="Z31" s="93"/>
+      <c r="AA31" s="93"/>
+      <c r="AB31" s="93"/>
+      <c r="AC31" s="93"/>
+      <c r="AD31" s="93"/>
+      <c r="AE31" s="93"/>
+      <c r="AF31" s="93"/>
+      <c r="AG31" s="93"/>
+      <c r="AH31" s="93"/>
+      <c r="AI31" s="93"/>
+      <c r="AJ31" s="93"/>
+      <c r="AK31" s="93"/>
+      <c r="AL31" s="93"/>
+      <c r="AM31" s="93"/>
+      <c r="AN31" s="93"/>
+      <c r="AO31" s="93"/>
+      <c r="AP31" s="93"/>
+      <c r="AQ31" s="93"/>
+      <c r="AR31" s="93"/>
+      <c r="AS31" s="93"/>
+      <c r="AT31" s="93"/>
+      <c r="AU31" s="93"/>
+      <c r="AV31" s="93"/>
+      <c r="AW31" s="93"/>
+      <c r="AX31" s="93"/>
+      <c r="AY31" s="93"/>
+      <c r="AZ31" s="93"/>
+      <c r="BA31" s="93"/>
+      <c r="BB31" s="93"/>
+      <c r="BC31" s="93"/>
+      <c r="BD31" s="93"/>
+      <c r="BE31" s="93"/>
+      <c r="BF31" s="93"/>
+      <c r="BG31" s="93"/>
+      <c r="BH31" s="93"/>
+      <c r="BI31" s="93"/>
+      <c r="BJ31" s="93"/>
+      <c r="BK31" s="93"/>
+      <c r="BL31" s="93"/>
+      <c r="BM31" s="93"/>
+      <c r="BN31" s="93"/>
+      <c r="BO31" s="93"/>
+      <c r="BP31" s="93"/>
+      <c r="BQ31" s="93"/>
+      <c r="BR31" s="93"/>
+      <c r="BS31" s="93"/>
+      <c r="BT31" s="93"/>
+      <c r="BU31" s="93"/>
+      <c r="BV31" s="93"/>
+      <c r="BW31" s="93"/>
+      <c r="BX31" s="93"/>
+      <c r="BY31" s="93"/>
+      <c r="BZ31" s="93"/>
+      <c r="CA31" s="93"/>
+      <c r="CB31" s="93"/>
+      <c r="CC31" s="93"/>
+      <c r="CD31" s="93"/>
+      <c r="CE31" s="93"/>
+      <c r="CF31" s="93"/>
+      <c r="CG31" s="93"/>
+      <c r="CH31" s="93"/>
+      <c r="CI31" s="93"/>
+      <c r="CJ31" s="93"/>
+      <c r="CK31" s="93"/>
+      <c r="CL31" s="93"/>
+      <c r="CM31" s="93"/>
+      <c r="CN31" s="93"/>
+      <c r="CO31" s="93"/>
+      <c r="CP31" s="93"/>
+      <c r="CQ31" s="93"/>
+      <c r="CR31" s="93"/>
+      <c r="CS31" s="93"/>
+      <c r="CT31" s="93"/>
+      <c r="CU31" s="93"/>
+      <c r="CV31" s="93"/>
+      <c r="CW31" s="93"/>
+      <c r="CX31" s="93"/>
+      <c r="CY31" s="93"/>
+      <c r="CZ31" s="93"/>
+      <c r="DA31" s="93"/>
+      <c r="DB31" s="93"/>
+      <c r="DC31" s="93"/>
+      <c r="DD31" s="93"/>
+      <c r="DE31" s="93"/>
+      <c r="DF31" s="93"/>
+      <c r="DG31" s="93"/>
+      <c r="DH31" s="93"/>
+      <c r="DI31" s="93"/>
+      <c r="DJ31" s="93"/>
+      <c r="DK31" s="93"/>
+      <c r="DL31" s="93"/>
+      <c r="DM31" s="93"/>
+      <c r="DN31" s="93"/>
+      <c r="DO31" s="93"/>
+      <c r="DP31" s="93"/>
+      <c r="DQ31" s="93"/>
+    </row>
+    <row r="32" spans="1:121" ht="22">
       <c r="A32" s="4"/>
       <c r="B32" s="3">
         <v>5</v>
@@ -1898,8 +3302,119 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="12"/>
-    </row>
-    <row r="33" spans="1:10" ht="22">
+      <c r="K32" s="93"/>
+      <c r="L32" s="93"/>
+      <c r="M32" s="93"/>
+      <c r="N32" s="93"/>
+      <c r="O32" s="93"/>
+      <c r="P32" s="93"/>
+      <c r="Q32" s="93"/>
+      <c r="R32" s="93"/>
+      <c r="S32" s="93"/>
+      <c r="T32" s="93"/>
+      <c r="U32" s="93"/>
+      <c r="V32" s="93"/>
+      <c r="W32" s="93"/>
+      <c r="X32" s="93"/>
+      <c r="Y32" s="93"/>
+      <c r="Z32" s="93"/>
+      <c r="AA32" s="93"/>
+      <c r="AB32" s="93"/>
+      <c r="AC32" s="93"/>
+      <c r="AD32" s="93"/>
+      <c r="AE32" s="93"/>
+      <c r="AF32" s="93"/>
+      <c r="AG32" s="93"/>
+      <c r="AH32" s="93"/>
+      <c r="AI32" s="93"/>
+      <c r="AJ32" s="93"/>
+      <c r="AK32" s="93"/>
+      <c r="AL32" s="93"/>
+      <c r="AM32" s="93"/>
+      <c r="AN32" s="93"/>
+      <c r="AO32" s="93"/>
+      <c r="AP32" s="93"/>
+      <c r="AQ32" s="93"/>
+      <c r="AR32" s="93"/>
+      <c r="AS32" s="93"/>
+      <c r="AT32" s="93"/>
+      <c r="AU32" s="93"/>
+      <c r="AV32" s="93"/>
+      <c r="AW32" s="93"/>
+      <c r="AX32" s="93"/>
+      <c r="AY32" s="93"/>
+      <c r="AZ32" s="93"/>
+      <c r="BA32" s="93"/>
+      <c r="BB32" s="93"/>
+      <c r="BC32" s="93"/>
+      <c r="BD32" s="93"/>
+      <c r="BE32" s="93"/>
+      <c r="BF32" s="93"/>
+      <c r="BG32" s="93"/>
+      <c r="BH32" s="93"/>
+      <c r="BI32" s="93"/>
+      <c r="BJ32" s="93"/>
+      <c r="BK32" s="93"/>
+      <c r="BL32" s="93"/>
+      <c r="BM32" s="93"/>
+      <c r="BN32" s="93"/>
+      <c r="BO32" s="93"/>
+      <c r="BP32" s="93"/>
+      <c r="BQ32" s="93"/>
+      <c r="BR32" s="93"/>
+      <c r="BS32" s="93"/>
+      <c r="BT32" s="93"/>
+      <c r="BU32" s="93"/>
+      <c r="BV32" s="93"/>
+      <c r="BW32" s="93"/>
+      <c r="BX32" s="93"/>
+      <c r="BY32" s="93"/>
+      <c r="BZ32" s="93"/>
+      <c r="CA32" s="93"/>
+      <c r="CB32" s="93"/>
+      <c r="CC32" s="93"/>
+      <c r="CD32" s="93"/>
+      <c r="CE32" s="93"/>
+      <c r="CF32" s="93"/>
+      <c r="CG32" s="93"/>
+      <c r="CH32" s="93"/>
+      <c r="CI32" s="93"/>
+      <c r="CJ32" s="93"/>
+      <c r="CK32" s="93"/>
+      <c r="CL32" s="93"/>
+      <c r="CM32" s="93"/>
+      <c r="CN32" s="93"/>
+      <c r="CO32" s="93"/>
+      <c r="CP32" s="93"/>
+      <c r="CQ32" s="93"/>
+      <c r="CR32" s="93"/>
+      <c r="CS32" s="93"/>
+      <c r="CT32" s="93"/>
+      <c r="CU32" s="93"/>
+      <c r="CV32" s="93"/>
+      <c r="CW32" s="93"/>
+      <c r="CX32" s="93"/>
+      <c r="CY32" s="93"/>
+      <c r="CZ32" s="93"/>
+      <c r="DA32" s="93"/>
+      <c r="DB32" s="93"/>
+      <c r="DC32" s="93"/>
+      <c r="DD32" s="93"/>
+      <c r="DE32" s="93"/>
+      <c r="DF32" s="93"/>
+      <c r="DG32" s="93"/>
+      <c r="DH32" s="93"/>
+      <c r="DI32" s="93"/>
+      <c r="DJ32" s="93"/>
+      <c r="DK32" s="93"/>
+      <c r="DL32" s="93"/>
+      <c r="DM32" s="93"/>
+      <c r="DN32" s="93"/>
+      <c r="DO32" s="93"/>
+      <c r="DP32" s="93"/>
+      <c r="DQ32" s="93"/>
+    </row>
+    <row r="33" spans="1:121" ht="22">
       <c r="A33" s="3" t="s">
         <v>12</v>
       </c>
@@ -1920,8 +3435,119 @@
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="12"/>
-    </row>
-    <row r="34" spans="1:10" ht="22">
+      <c r="K33" s="93"/>
+      <c r="L33" s="93"/>
+      <c r="M33" s="93"/>
+      <c r="N33" s="93"/>
+      <c r="O33" s="93"/>
+      <c r="P33" s="93"/>
+      <c r="Q33" s="93"/>
+      <c r="R33" s="93"/>
+      <c r="S33" s="93"/>
+      <c r="T33" s="93"/>
+      <c r="U33" s="93"/>
+      <c r="V33" s="93"/>
+      <c r="W33" s="93"/>
+      <c r="X33" s="93"/>
+      <c r="Y33" s="93"/>
+      <c r="Z33" s="93"/>
+      <c r="AA33" s="93"/>
+      <c r="AB33" s="93"/>
+      <c r="AC33" s="93"/>
+      <c r="AD33" s="93"/>
+      <c r="AE33" s="93"/>
+      <c r="AF33" s="93"/>
+      <c r="AG33" s="93"/>
+      <c r="AH33" s="93"/>
+      <c r="AI33" s="93"/>
+      <c r="AJ33" s="93"/>
+      <c r="AK33" s="93"/>
+      <c r="AL33" s="93"/>
+      <c r="AM33" s="93"/>
+      <c r="AN33" s="93"/>
+      <c r="AO33" s="93"/>
+      <c r="AP33" s="93"/>
+      <c r="AQ33" s="93"/>
+      <c r="AR33" s="93"/>
+      <c r="AS33" s="93"/>
+      <c r="AT33" s="93"/>
+      <c r="AU33" s="93"/>
+      <c r="AV33" s="93"/>
+      <c r="AW33" s="93"/>
+      <c r="AX33" s="93"/>
+      <c r="AY33" s="93"/>
+      <c r="AZ33" s="93"/>
+      <c r="BA33" s="93"/>
+      <c r="BB33" s="93"/>
+      <c r="BC33" s="93"/>
+      <c r="BD33" s="93"/>
+      <c r="BE33" s="93"/>
+      <c r="BF33" s="93"/>
+      <c r="BG33" s="93"/>
+      <c r="BH33" s="93"/>
+      <c r="BI33" s="93"/>
+      <c r="BJ33" s="93"/>
+      <c r="BK33" s="93"/>
+      <c r="BL33" s="93"/>
+      <c r="BM33" s="93"/>
+      <c r="BN33" s="93"/>
+      <c r="BO33" s="93"/>
+      <c r="BP33" s="93"/>
+      <c r="BQ33" s="93"/>
+      <c r="BR33" s="93"/>
+      <c r="BS33" s="93"/>
+      <c r="BT33" s="93"/>
+      <c r="BU33" s="93"/>
+      <c r="BV33" s="93"/>
+      <c r="BW33" s="93"/>
+      <c r="BX33" s="93"/>
+      <c r="BY33" s="93"/>
+      <c r="BZ33" s="93"/>
+      <c r="CA33" s="93"/>
+      <c r="CB33" s="93"/>
+      <c r="CC33" s="93"/>
+      <c r="CD33" s="93"/>
+      <c r="CE33" s="93"/>
+      <c r="CF33" s="93"/>
+      <c r="CG33" s="93"/>
+      <c r="CH33" s="93"/>
+      <c r="CI33" s="93"/>
+      <c r="CJ33" s="93"/>
+      <c r="CK33" s="93"/>
+      <c r="CL33" s="93"/>
+      <c r="CM33" s="93"/>
+      <c r="CN33" s="93"/>
+      <c r="CO33" s="93"/>
+      <c r="CP33" s="93"/>
+      <c r="CQ33" s="93"/>
+      <c r="CR33" s="93"/>
+      <c r="CS33" s="93"/>
+      <c r="CT33" s="93"/>
+      <c r="CU33" s="93"/>
+      <c r="CV33" s="93"/>
+      <c r="CW33" s="93"/>
+      <c r="CX33" s="93"/>
+      <c r="CY33" s="93"/>
+      <c r="CZ33" s="93"/>
+      <c r="DA33" s="93"/>
+      <c r="DB33" s="93"/>
+      <c r="DC33" s="93"/>
+      <c r="DD33" s="93"/>
+      <c r="DE33" s="93"/>
+      <c r="DF33" s="93"/>
+      <c r="DG33" s="93"/>
+      <c r="DH33" s="93"/>
+      <c r="DI33" s="93"/>
+      <c r="DJ33" s="93"/>
+      <c r="DK33" s="93"/>
+      <c r="DL33" s="93"/>
+      <c r="DM33" s="93"/>
+      <c r="DN33" s="93"/>
+      <c r="DO33" s="93"/>
+      <c r="DP33" s="93"/>
+      <c r="DQ33" s="93"/>
+    </row>
+    <row r="34" spans="1:121" ht="22">
       <c r="A34" s="61" t="s">
         <v>17</v>
       </c>
@@ -1950,7 +3576,7 @@
       <c r="I34" s="64"/>
       <c r="J34" s="65"/>
     </row>
-    <row r="35" spans="1:10" ht="24">
+    <row r="35" spans="1:121" ht="24">
       <c r="A35" s="62"/>
       <c r="B35" s="16" t="s">
         <v>26</v>
@@ -1970,7 +3596,7 @@
       <c r="I35" s="88"/>
       <c r="J35" s="89"/>
     </row>
-    <row r="36" spans="1:10" ht="22" customHeight="1">
+    <row r="36" spans="1:121" ht="22" customHeight="1">
       <c r="A36" s="74"/>
       <c r="B36" s="16"/>
       <c r="C36" s="50">
@@ -1988,7 +3614,7 @@
       <c r="I36" s="77"/>
       <c r="J36" s="78"/>
     </row>
-    <row r="37" spans="1:10" ht="22" customHeight="1">
+    <row r="37" spans="1:121" ht="22" customHeight="1">
       <c r="A37" s="75"/>
       <c r="B37" s="16"/>
       <c r="C37" s="53"/>
@@ -2000,7 +3626,7 @@
       <c r="I37" s="80"/>
       <c r="J37" s="81"/>
     </row>
-    <row r="38" spans="1:10" s="29" customFormat="1" ht="11">
+    <row r="38" spans="1:121" s="29" customFormat="1" ht="11">
       <c r="A38" s="56"/>
       <c r="B38" s="57"/>
       <c r="C38" s="57"/>
@@ -2012,7 +3638,7 @@
       <c r="I38" s="57"/>
       <c r="J38" s="58"/>
     </row>
-    <row r="39" spans="1:10" ht="22">
+    <row r="39" spans="1:121" ht="22">
       <c r="A39" s="3" t="s">
         <v>3</v>
       </c>
@@ -2040,7 +3666,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="9"/>
     </row>
-    <row r="40" spans="1:10" ht="22">
+    <row r="40" spans="1:121" ht="22">
       <c r="A40" s="17"/>
       <c r="B40" s="3" t="s">
         <v>8</v>
@@ -2064,7 +3690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="22">
+    <row r="41" spans="1:121" ht="22">
       <c r="A41" s="3" t="s">
         <v>10</v>
       </c>
@@ -2087,8 +3713,47 @@
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="12"/>
-    </row>
-    <row r="42" spans="1:10" ht="22">
+      <c r="K41" s="93"/>
+      <c r="L41" s="93"/>
+      <c r="M41" s="93"/>
+      <c r="N41" s="93"/>
+      <c r="O41" s="93"/>
+      <c r="P41" s="93"/>
+      <c r="Q41" s="93"/>
+      <c r="R41" s="93"/>
+      <c r="S41" s="93"/>
+      <c r="T41" s="93"/>
+      <c r="U41" s="93"/>
+      <c r="V41" s="93"/>
+      <c r="W41" s="93"/>
+      <c r="X41" s="93"/>
+      <c r="Y41" s="93"/>
+      <c r="Z41" s="93"/>
+      <c r="AA41" s="93"/>
+      <c r="AB41" s="93"/>
+      <c r="AC41" s="93"/>
+      <c r="AD41" s="93"/>
+      <c r="AE41" s="93"/>
+      <c r="AF41" s="93"/>
+      <c r="AG41" s="93"/>
+      <c r="AH41" s="93"/>
+      <c r="AI41" s="93"/>
+      <c r="AJ41" s="93"/>
+      <c r="AK41" s="93"/>
+      <c r="AL41" s="93"/>
+      <c r="AM41" s="93"/>
+      <c r="AN41" s="93"/>
+      <c r="AO41" s="93"/>
+      <c r="AP41" s="93"/>
+      <c r="AQ41" s="93"/>
+      <c r="AR41" s="93"/>
+      <c r="AS41" s="93"/>
+      <c r="AT41" s="93"/>
+      <c r="AU41" s="93"/>
+      <c r="AV41" s="93"/>
+      <c r="AW41" s="93"/>
+    </row>
+    <row r="42" spans="1:121" ht="22">
       <c r="A42" s="3" t="s">
         <v>11</v>
       </c>
@@ -2117,8 +3782,47 @@
       <c r="J42" s="12">
         <v>19</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" ht="22">
+      <c r="K42" s="93"/>
+      <c r="L42" s="93"/>
+      <c r="M42" s="93"/>
+      <c r="N42" s="93"/>
+      <c r="O42" s="93"/>
+      <c r="P42" s="93"/>
+      <c r="Q42" s="93"/>
+      <c r="R42" s="93"/>
+      <c r="S42" s="93"/>
+      <c r="T42" s="93"/>
+      <c r="U42" s="93"/>
+      <c r="V42" s="93"/>
+      <c r="W42" s="93"/>
+      <c r="X42" s="93"/>
+      <c r="Y42" s="93"/>
+      <c r="Z42" s="93"/>
+      <c r="AA42" s="93"/>
+      <c r="AB42" s="93"/>
+      <c r="AC42" s="93"/>
+      <c r="AD42" s="93"/>
+      <c r="AE42" s="93"/>
+      <c r="AF42" s="93"/>
+      <c r="AG42" s="93"/>
+      <c r="AH42" s="93"/>
+      <c r="AI42" s="93"/>
+      <c r="AJ42" s="93"/>
+      <c r="AK42" s="93"/>
+      <c r="AL42" s="93"/>
+      <c r="AM42" s="93"/>
+      <c r="AN42" s="93"/>
+      <c r="AO42" s="93"/>
+      <c r="AP42" s="93"/>
+      <c r="AQ42" s="93"/>
+      <c r="AR42" s="93"/>
+      <c r="AS42" s="93"/>
+      <c r="AT42" s="93"/>
+      <c r="AU42" s="93"/>
+      <c r="AV42" s="93"/>
+      <c r="AW42" s="93"/>
+    </row>
+    <row r="43" spans="1:121" ht="22">
       <c r="A43" s="4"/>
       <c r="B43" s="3">
         <v>3</v>
@@ -2141,8 +3845,47 @@
       </c>
       <c r="I43" s="4"/>
       <c r="J43" s="12"/>
-    </row>
-    <row r="44" spans="1:10" ht="22">
+      <c r="K43" s="93"/>
+      <c r="L43" s="93"/>
+      <c r="M43" s="93"/>
+      <c r="N43" s="93"/>
+      <c r="O43" s="93"/>
+      <c r="P43" s="93"/>
+      <c r="Q43" s="93"/>
+      <c r="R43" s="93"/>
+      <c r="S43" s="93"/>
+      <c r="T43" s="93"/>
+      <c r="U43" s="93"/>
+      <c r="V43" s="93"/>
+      <c r="W43" s="93"/>
+      <c r="X43" s="93"/>
+      <c r="Y43" s="93"/>
+      <c r="Z43" s="93"/>
+      <c r="AA43" s="93"/>
+      <c r="AB43" s="93"/>
+      <c r="AC43" s="93"/>
+      <c r="AD43" s="93"/>
+      <c r="AE43" s="93"/>
+      <c r="AF43" s="93"/>
+      <c r="AG43" s="93"/>
+      <c r="AH43" s="93"/>
+      <c r="AI43" s="93"/>
+      <c r="AJ43" s="93"/>
+      <c r="AK43" s="93"/>
+      <c r="AL43" s="93"/>
+      <c r="AM43" s="93"/>
+      <c r="AN43" s="93"/>
+      <c r="AO43" s="93"/>
+      <c r="AP43" s="93"/>
+      <c r="AQ43" s="93"/>
+      <c r="AR43" s="93"/>
+      <c r="AS43" s="93"/>
+      <c r="AT43" s="93"/>
+      <c r="AU43" s="93"/>
+      <c r="AV43" s="93"/>
+      <c r="AW43" s="93"/>
+    </row>
+    <row r="44" spans="1:121" ht="22">
       <c r="A44" s="4"/>
       <c r="B44" s="3">
         <v>4</v>
@@ -2169,8 +3912,47 @@
       <c r="J44" s="12">
         <v>940</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" ht="22">
+      <c r="K44" s="93"/>
+      <c r="L44" s="93"/>
+      <c r="M44" s="93"/>
+      <c r="N44" s="93"/>
+      <c r="O44" s="93"/>
+      <c r="P44" s="93"/>
+      <c r="Q44" s="93"/>
+      <c r="R44" s="93"/>
+      <c r="S44" s="93"/>
+      <c r="T44" s="93"/>
+      <c r="U44" s="93"/>
+      <c r="V44" s="93"/>
+      <c r="W44" s="93"/>
+      <c r="X44" s="93"/>
+      <c r="Y44" s="93"/>
+      <c r="Z44" s="93"/>
+      <c r="AA44" s="93"/>
+      <c r="AB44" s="93"/>
+      <c r="AC44" s="93"/>
+      <c r="AD44" s="93"/>
+      <c r="AE44" s="93"/>
+      <c r="AF44" s="93"/>
+      <c r="AG44" s="93"/>
+      <c r="AH44" s="93"/>
+      <c r="AI44" s="93"/>
+      <c r="AJ44" s="93"/>
+      <c r="AK44" s="93"/>
+      <c r="AL44" s="93"/>
+      <c r="AM44" s="93"/>
+      <c r="AN44" s="93"/>
+      <c r="AO44" s="93"/>
+      <c r="AP44" s="93"/>
+      <c r="AQ44" s="93"/>
+      <c r="AR44" s="93"/>
+      <c r="AS44" s="93"/>
+      <c r="AT44" s="93"/>
+      <c r="AU44" s="93"/>
+      <c r="AV44" s="93"/>
+      <c r="AW44" s="93"/>
+    </row>
+    <row r="45" spans="1:121" ht="22">
       <c r="A45" s="4"/>
       <c r="B45" s="3">
         <v>5</v>
@@ -2197,8 +3979,47 @@
       <c r="J45" s="12">
         <v>332</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" ht="22">
+      <c r="K45" s="93"/>
+      <c r="L45" s="93"/>
+      <c r="M45" s="93"/>
+      <c r="N45" s="93"/>
+      <c r="O45" s="93"/>
+      <c r="P45" s="93"/>
+      <c r="Q45" s="93"/>
+      <c r="R45" s="93"/>
+      <c r="S45" s="93"/>
+      <c r="T45" s="93"/>
+      <c r="U45" s="93"/>
+      <c r="V45" s="93"/>
+      <c r="W45" s="93"/>
+      <c r="X45" s="93"/>
+      <c r="Y45" s="93"/>
+      <c r="Z45" s="93"/>
+      <c r="AA45" s="93"/>
+      <c r="AB45" s="93"/>
+      <c r="AC45" s="93"/>
+      <c r="AD45" s="93"/>
+      <c r="AE45" s="93"/>
+      <c r="AF45" s="93"/>
+      <c r="AG45" s="93"/>
+      <c r="AH45" s="93"/>
+      <c r="AI45" s="93"/>
+      <c r="AJ45" s="93"/>
+      <c r="AK45" s="93"/>
+      <c r="AL45" s="93"/>
+      <c r="AM45" s="93"/>
+      <c r="AN45" s="93"/>
+      <c r="AO45" s="93"/>
+      <c r="AP45" s="93"/>
+      <c r="AQ45" s="93"/>
+      <c r="AR45" s="93"/>
+      <c r="AS45" s="93"/>
+      <c r="AT45" s="93"/>
+      <c r="AU45" s="93"/>
+      <c r="AV45" s="93"/>
+      <c r="AW45" s="93"/>
+    </row>
+    <row r="46" spans="1:121" ht="22">
       <c r="A46" s="3" t="s">
         <v>12</v>
       </c>
@@ -2215,8 +4036,47 @@
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="J46" s="12"/>
-    </row>
-    <row r="47" spans="1:10" ht="22">
+      <c r="K46" s="93"/>
+      <c r="L46" s="93"/>
+      <c r="M46" s="93"/>
+      <c r="N46" s="93"/>
+      <c r="O46" s="93"/>
+      <c r="P46" s="93"/>
+      <c r="Q46" s="93"/>
+      <c r="R46" s="93"/>
+      <c r="S46" s="93"/>
+      <c r="T46" s="93"/>
+      <c r="U46" s="93"/>
+      <c r="V46" s="93"/>
+      <c r="W46" s="93"/>
+      <c r="X46" s="93"/>
+      <c r="Y46" s="93"/>
+      <c r="Z46" s="93"/>
+      <c r="AA46" s="93"/>
+      <c r="AB46" s="93"/>
+      <c r="AC46" s="93"/>
+      <c r="AD46" s="93"/>
+      <c r="AE46" s="93"/>
+      <c r="AF46" s="93"/>
+      <c r="AG46" s="93"/>
+      <c r="AH46" s="93"/>
+      <c r="AI46" s="93"/>
+      <c r="AJ46" s="93"/>
+      <c r="AK46" s="93"/>
+      <c r="AL46" s="93"/>
+      <c r="AM46" s="93"/>
+      <c r="AN46" s="93"/>
+      <c r="AO46" s="93"/>
+      <c r="AP46" s="93"/>
+      <c r="AQ46" s="93"/>
+      <c r="AR46" s="93"/>
+      <c r="AS46" s="93"/>
+      <c r="AT46" s="93"/>
+      <c r="AU46" s="93"/>
+      <c r="AV46" s="93"/>
+      <c r="AW46" s="93"/>
+    </row>
+    <row r="47" spans="1:121" ht="22">
       <c r="A47" s="90" t="s">
         <v>18</v>
       </c>
@@ -2245,7 +4105,7 @@
       <c r="I47" s="64"/>
       <c r="J47" s="65"/>
     </row>
-    <row r="48" spans="1:10" ht="22">
+    <row r="48" spans="1:121" ht="22">
       <c r="A48" s="91"/>
       <c r="B48" s="16" t="s">
         <v>26</v>
@@ -2265,7 +4125,7 @@
       <c r="I48" s="64"/>
       <c r="J48" s="65"/>
     </row>
-    <row r="49" spans="1:10" ht="22" customHeight="1">
+    <row r="49" spans="1:47" ht="22" customHeight="1">
       <c r="A49" s="68"/>
       <c r="B49" s="66" t="s">
         <v>28</v>
@@ -2285,7 +4145,7 @@
       <c r="I49" s="42"/>
       <c r="J49" s="43"/>
     </row>
-    <row r="50" spans="1:10" ht="22" customHeight="1">
+    <row r="50" spans="1:47" ht="22" customHeight="1">
       <c r="A50" s="69"/>
       <c r="B50" s="67"/>
       <c r="C50" s="44"/>
@@ -2297,7 +4157,7 @@
       <c r="I50" s="45"/>
       <c r="J50" s="46"/>
     </row>
-    <row r="51" spans="1:10" s="29" customFormat="1" ht="11">
+    <row r="51" spans="1:47" s="29" customFormat="1" ht="11">
       <c r="A51" s="56"/>
       <c r="B51" s="57"/>
       <c r="C51" s="57"/>
@@ -2309,7 +4169,7 @@
       <c r="I51" s="57"/>
       <c r="J51" s="58"/>
     </row>
-    <row r="52" spans="1:10" ht="22">
+    <row r="52" spans="1:47" ht="22">
       <c r="A52" s="3" t="s">
         <v>3</v>
       </c>
@@ -2337,7 +4197,7 @@
       <c r="I52" s="8"/>
       <c r="J52" s="9"/>
     </row>
-    <row r="53" spans="1:10" ht="22">
+    <row r="53" spans="1:47" ht="22">
       <c r="A53" s="10"/>
       <c r="B53" s="3" t="s">
         <v>8</v>
@@ -2361,7 +4221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="22">
+    <row r="54" spans="1:47" ht="22">
       <c r="A54" s="4"/>
       <c r="B54" s="3">
         <v>1</v>
@@ -2382,8 +4242,45 @@
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="J54" s="12"/>
-    </row>
-    <row r="55" spans="1:10" ht="22">
+      <c r="K54" s="93"/>
+      <c r="L54" s="93"/>
+      <c r="M54" s="93"/>
+      <c r="N54" s="93"/>
+      <c r="O54" s="93"/>
+      <c r="P54" s="93"/>
+      <c r="Q54" s="93"/>
+      <c r="R54" s="93"/>
+      <c r="S54" s="93"/>
+      <c r="T54" s="93"/>
+      <c r="U54" s="93"/>
+      <c r="V54" s="93"/>
+      <c r="W54" s="93"/>
+      <c r="X54" s="93"/>
+      <c r="Y54" s="93"/>
+      <c r="Z54" s="93"/>
+      <c r="AA54" s="93"/>
+      <c r="AB54" s="93"/>
+      <c r="AC54" s="93"/>
+      <c r="AD54" s="93"/>
+      <c r="AE54" s="93"/>
+      <c r="AF54" s="93"/>
+      <c r="AG54" s="93"/>
+      <c r="AH54" s="93"/>
+      <c r="AI54" s="93"/>
+      <c r="AJ54" s="93"/>
+      <c r="AK54" s="93"/>
+      <c r="AL54" s="93"/>
+      <c r="AM54" s="93"/>
+      <c r="AN54" s="93"/>
+      <c r="AO54" s="93"/>
+      <c r="AP54" s="93"/>
+      <c r="AQ54" s="93"/>
+      <c r="AR54" s="93"/>
+      <c r="AS54" s="93"/>
+      <c r="AT54" s="93"/>
+      <c r="AU54" s="93"/>
+    </row>
+    <row r="55" spans="1:47" ht="22">
       <c r="A55" s="3" t="s">
         <v>10</v>
       </c>
@@ -2406,8 +4303,45 @@
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="J55" s="12"/>
-    </row>
-    <row r="56" spans="1:10" ht="22">
+      <c r="K55" s="93"/>
+      <c r="L55" s="93"/>
+      <c r="M55" s="93"/>
+      <c r="N55" s="93"/>
+      <c r="O55" s="93"/>
+      <c r="P55" s="93"/>
+      <c r="Q55" s="93"/>
+      <c r="R55" s="93"/>
+      <c r="S55" s="93"/>
+      <c r="T55" s="93"/>
+      <c r="U55" s="93"/>
+      <c r="V55" s="93"/>
+      <c r="W55" s="93"/>
+      <c r="X55" s="93"/>
+      <c r="Y55" s="93"/>
+      <c r="Z55" s="93"/>
+      <c r="AA55" s="93"/>
+      <c r="AB55" s="93"/>
+      <c r="AC55" s="93"/>
+      <c r="AD55" s="93"/>
+      <c r="AE55" s="93"/>
+      <c r="AF55" s="93"/>
+      <c r="AG55" s="93"/>
+      <c r="AH55" s="93"/>
+      <c r="AI55" s="93"/>
+      <c r="AJ55" s="93"/>
+      <c r="AK55" s="93"/>
+      <c r="AL55" s="93"/>
+      <c r="AM55" s="93"/>
+      <c r="AN55" s="93"/>
+      <c r="AO55" s="93"/>
+      <c r="AP55" s="93"/>
+      <c r="AQ55" s="93"/>
+      <c r="AR55" s="93"/>
+      <c r="AS55" s="93"/>
+      <c r="AT55" s="93"/>
+      <c r="AU55" s="93"/>
+    </row>
+    <row r="56" spans="1:47" ht="22">
       <c r="A56" s="3" t="s">
         <v>11</v>
       </c>
@@ -2434,8 +4368,45 @@
         <v>947</v>
       </c>
       <c r="J56" s="12"/>
-    </row>
-    <row r="57" spans="1:10" ht="22">
+      <c r="K56" s="93"/>
+      <c r="L56" s="93"/>
+      <c r="M56" s="93"/>
+      <c r="N56" s="93"/>
+      <c r="O56" s="93"/>
+      <c r="P56" s="93"/>
+      <c r="Q56" s="93"/>
+      <c r="R56" s="93"/>
+      <c r="S56" s="93"/>
+      <c r="T56" s="93"/>
+      <c r="U56" s="93"/>
+      <c r="V56" s="93"/>
+      <c r="W56" s="93"/>
+      <c r="X56" s="93"/>
+      <c r="Y56" s="93"/>
+      <c r="Z56" s="93"/>
+      <c r="AA56" s="93"/>
+      <c r="AB56" s="93"/>
+      <c r="AC56" s="93"/>
+      <c r="AD56" s="93"/>
+      <c r="AE56" s="93"/>
+      <c r="AF56" s="93"/>
+      <c r="AG56" s="93"/>
+      <c r="AH56" s="93"/>
+      <c r="AI56" s="93"/>
+      <c r="AJ56" s="93"/>
+      <c r="AK56" s="93"/>
+      <c r="AL56" s="93"/>
+      <c r="AM56" s="93"/>
+      <c r="AN56" s="93"/>
+      <c r="AO56" s="93"/>
+      <c r="AP56" s="93"/>
+      <c r="AQ56" s="93"/>
+      <c r="AR56" s="93"/>
+      <c r="AS56" s="93"/>
+      <c r="AT56" s="93"/>
+      <c r="AU56" s="93"/>
+    </row>
+    <row r="57" spans="1:47" ht="22">
       <c r="A57" s="4"/>
       <c r="B57" s="3">
         <v>4</v>
@@ -2458,8 +4429,45 @@
         <v>15</v>
       </c>
       <c r="J57" s="12"/>
-    </row>
-    <row r="58" spans="1:10" ht="22">
+      <c r="K57" s="93"/>
+      <c r="L57" s="93"/>
+      <c r="M57" s="93"/>
+      <c r="N57" s="93"/>
+      <c r="O57" s="93"/>
+      <c r="P57" s="93"/>
+      <c r="Q57" s="93"/>
+      <c r="R57" s="93"/>
+      <c r="S57" s="93"/>
+      <c r="T57" s="93"/>
+      <c r="U57" s="93"/>
+      <c r="V57" s="93"/>
+      <c r="W57" s="93"/>
+      <c r="X57" s="93"/>
+      <c r="Y57" s="93"/>
+      <c r="Z57" s="93"/>
+      <c r="AA57" s="93"/>
+      <c r="AB57" s="93"/>
+      <c r="AC57" s="93"/>
+      <c r="AD57" s="93"/>
+      <c r="AE57" s="93"/>
+      <c r="AF57" s="93"/>
+      <c r="AG57" s="93"/>
+      <c r="AH57" s="93"/>
+      <c r="AI57" s="93"/>
+      <c r="AJ57" s="93"/>
+      <c r="AK57" s="93"/>
+      <c r="AL57" s="93"/>
+      <c r="AM57" s="93"/>
+      <c r="AN57" s="93"/>
+      <c r="AO57" s="93"/>
+      <c r="AP57" s="93"/>
+      <c r="AQ57" s="93"/>
+      <c r="AR57" s="93"/>
+      <c r="AS57" s="93"/>
+      <c r="AT57" s="93"/>
+      <c r="AU57" s="93"/>
+    </row>
+    <row r="58" spans="1:47" ht="22">
       <c r="A58" s="4"/>
       <c r="B58" s="3">
         <v>5</v>
@@ -2486,8 +4494,45 @@
       <c r="J58" s="12">
         <v>337</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" ht="22">
+      <c r="K58" s="93"/>
+      <c r="L58" s="93"/>
+      <c r="M58" s="93"/>
+      <c r="N58" s="93"/>
+      <c r="O58" s="93"/>
+      <c r="P58" s="93"/>
+      <c r="Q58" s="93"/>
+      <c r="R58" s="93"/>
+      <c r="S58" s="93"/>
+      <c r="T58" s="93"/>
+      <c r="U58" s="93"/>
+      <c r="V58" s="93"/>
+      <c r="W58" s="93"/>
+      <c r="X58" s="93"/>
+      <c r="Y58" s="93"/>
+      <c r="Z58" s="93"/>
+      <c r="AA58" s="93"/>
+      <c r="AB58" s="93"/>
+      <c r="AC58" s="93"/>
+      <c r="AD58" s="93"/>
+      <c r="AE58" s="93"/>
+      <c r="AF58" s="93"/>
+      <c r="AG58" s="93"/>
+      <c r="AH58" s="93"/>
+      <c r="AI58" s="93"/>
+      <c r="AJ58" s="93"/>
+      <c r="AK58" s="93"/>
+      <c r="AL58" s="93"/>
+      <c r="AM58" s="93"/>
+      <c r="AN58" s="93"/>
+      <c r="AO58" s="93"/>
+      <c r="AP58" s="93"/>
+      <c r="AQ58" s="93"/>
+      <c r="AR58" s="93"/>
+      <c r="AS58" s="93"/>
+      <c r="AT58" s="93"/>
+      <c r="AU58" s="93"/>
+    </row>
+    <row r="59" spans="1:47" ht="22">
       <c r="A59" s="3" t="s">
         <v>12</v>
       </c>
@@ -2506,8 +4551,45 @@
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="J59" s="12"/>
-    </row>
-    <row r="60" spans="1:10" ht="22">
+      <c r="K59" s="93"/>
+      <c r="L59" s="93"/>
+      <c r="M59" s="93"/>
+      <c r="N59" s="93"/>
+      <c r="O59" s="93"/>
+      <c r="P59" s="93"/>
+      <c r="Q59" s="93"/>
+      <c r="R59" s="93"/>
+      <c r="S59" s="93"/>
+      <c r="T59" s="93"/>
+      <c r="U59" s="93"/>
+      <c r="V59" s="93"/>
+      <c r="W59" s="93"/>
+      <c r="X59" s="93"/>
+      <c r="Y59" s="93"/>
+      <c r="Z59" s="93"/>
+      <c r="AA59" s="93"/>
+      <c r="AB59" s="93"/>
+      <c r="AC59" s="93"/>
+      <c r="AD59" s="93"/>
+      <c r="AE59" s="93"/>
+      <c r="AF59" s="93"/>
+      <c r="AG59" s="93"/>
+      <c r="AH59" s="93"/>
+      <c r="AI59" s="93"/>
+      <c r="AJ59" s="93"/>
+      <c r="AK59" s="93"/>
+      <c r="AL59" s="93"/>
+      <c r="AM59" s="93"/>
+      <c r="AN59" s="93"/>
+      <c r="AO59" s="93"/>
+      <c r="AP59" s="93"/>
+      <c r="AQ59" s="93"/>
+      <c r="AR59" s="93"/>
+      <c r="AS59" s="93"/>
+      <c r="AT59" s="93"/>
+      <c r="AU59" s="93"/>
+    </row>
+    <row r="60" spans="1:47" ht="22">
       <c r="A60" s="90" t="s">
         <v>19</v>
       </c>
@@ -2536,7 +4618,7 @@
       <c r="I60" s="64"/>
       <c r="J60" s="65"/>
     </row>
-    <row r="61" spans="1:10" ht="24">
+    <row r="61" spans="1:47" ht="24">
       <c r="A61" s="91"/>
       <c r="B61" s="16" t="s">
         <v>26</v>
@@ -2556,7 +4638,7 @@
       <c r="I61" s="88"/>
       <c r="J61" s="89"/>
     </row>
-    <row r="62" spans="1:10" ht="22" customHeight="1">
+    <row r="62" spans="1:47" ht="22" customHeight="1">
       <c r="A62" s="74"/>
       <c r="B62" s="16"/>
       <c r="C62" s="50">
@@ -2574,7 +4656,7 @@
       <c r="I62" s="77"/>
       <c r="J62" s="78"/>
     </row>
-    <row r="63" spans="1:10" ht="22" customHeight="1">
+    <row r="63" spans="1:47" ht="22" customHeight="1">
       <c r="A63" s="75"/>
       <c r="B63" s="16"/>
       <c r="C63" s="53"/>
@@ -2586,7 +4668,7 @@
       <c r="I63" s="80"/>
       <c r="J63" s="81"/>
     </row>
-    <row r="64" spans="1:10" s="29" customFormat="1" ht="11">
+    <row r="64" spans="1:47" s="29" customFormat="1" ht="11">
       <c r="A64" s="56"/>
       <c r="B64" s="57"/>
       <c r="C64" s="57"/>
@@ -2598,7 +4680,7 @@
       <c r="I64" s="57"/>
       <c r="J64" s="58"/>
     </row>
-    <row r="65" spans="1:10" ht="22">
+    <row r="65" spans="1:90" ht="22">
       <c r="A65" s="3" t="s">
         <v>3</v>
       </c>
@@ -2626,7 +4708,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="9"/>
     </row>
-    <row r="66" spans="1:10" ht="22">
+    <row r="66" spans="1:90" ht="22">
       <c r="A66" s="17"/>
       <c r="B66" s="3" t="s">
         <v>8</v>
@@ -2650,7 +4732,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="22">
+    <row r="67" spans="1:90" ht="22">
       <c r="A67" s="4"/>
       <c r="B67" s="3">
         <v>1</v>
@@ -2671,8 +4753,40 @@
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
       <c r="J67" s="12"/>
-    </row>
-    <row r="68" spans="1:10" ht="22">
+      <c r="K67" s="93"/>
+      <c r="L67" s="93"/>
+      <c r="M67" s="93"/>
+      <c r="N67" s="93"/>
+      <c r="O67" s="93"/>
+      <c r="P67" s="93"/>
+      <c r="Q67" s="93"/>
+      <c r="R67" s="93"/>
+      <c r="S67" s="93"/>
+      <c r="T67" s="93"/>
+      <c r="U67" s="93"/>
+      <c r="V67" s="93"/>
+      <c r="W67" s="93"/>
+      <c r="X67" s="93"/>
+      <c r="Y67" s="93"/>
+      <c r="Z67" s="93"/>
+      <c r="AA67" s="93"/>
+      <c r="AB67" s="93"/>
+      <c r="AC67" s="93"/>
+      <c r="AD67" s="93"/>
+      <c r="AE67" s="93"/>
+      <c r="AF67" s="93"/>
+      <c r="AG67" s="93"/>
+      <c r="AH67" s="93"/>
+      <c r="AI67" s="93"/>
+      <c r="AJ67" s="93"/>
+      <c r="AK67" s="93"/>
+      <c r="AL67" s="93"/>
+      <c r="AM67" s="93"/>
+      <c r="AN67" s="93"/>
+      <c r="AO67" s="93"/>
+      <c r="AP67" s="93"/>
+    </row>
+    <row r="68" spans="1:90" ht="22">
       <c r="A68" s="3" t="s">
         <v>20</v>
       </c>
@@ -2701,8 +4815,40 @@
       <c r="J68" s="12">
         <v>951</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" ht="22">
+      <c r="K68" s="93"/>
+      <c r="L68" s="93"/>
+      <c r="M68" s="93"/>
+      <c r="N68" s="93"/>
+      <c r="O68" s="93"/>
+      <c r="P68" s="93"/>
+      <c r="Q68" s="93"/>
+      <c r="R68" s="93"/>
+      <c r="S68" s="93"/>
+      <c r="T68" s="93"/>
+      <c r="U68" s="93"/>
+      <c r="V68" s="93"/>
+      <c r="W68" s="93"/>
+      <c r="X68" s="93"/>
+      <c r="Y68" s="93"/>
+      <c r="Z68" s="93"/>
+      <c r="AA68" s="93"/>
+      <c r="AB68" s="93"/>
+      <c r="AC68" s="93"/>
+      <c r="AD68" s="93"/>
+      <c r="AE68" s="93"/>
+      <c r="AF68" s="93"/>
+      <c r="AG68" s="93"/>
+      <c r="AH68" s="93"/>
+      <c r="AI68" s="93"/>
+      <c r="AJ68" s="93"/>
+      <c r="AK68" s="93"/>
+      <c r="AL68" s="93"/>
+      <c r="AM68" s="93"/>
+      <c r="AN68" s="93"/>
+      <c r="AO68" s="93"/>
+      <c r="AP68" s="93"/>
+    </row>
+    <row r="69" spans="1:90" ht="22">
       <c r="A69" s="3" t="s">
         <v>11</v>
       </c>
@@ -2727,8 +4873,40 @@
         <v>11</v>
       </c>
       <c r="J69" s="12"/>
-    </row>
-    <row r="70" spans="1:10" ht="22">
+      <c r="K69" s="93"/>
+      <c r="L69" s="93"/>
+      <c r="M69" s="93"/>
+      <c r="N69" s="93"/>
+      <c r="O69" s="93"/>
+      <c r="P69" s="93"/>
+      <c r="Q69" s="93"/>
+      <c r="R69" s="93"/>
+      <c r="S69" s="93"/>
+      <c r="T69" s="93"/>
+      <c r="U69" s="93"/>
+      <c r="V69" s="93"/>
+      <c r="W69" s="93"/>
+      <c r="X69" s="93"/>
+      <c r="Y69" s="93"/>
+      <c r="Z69" s="93"/>
+      <c r="AA69" s="93"/>
+      <c r="AB69" s="93"/>
+      <c r="AC69" s="93"/>
+      <c r="AD69" s="93"/>
+      <c r="AE69" s="93"/>
+      <c r="AF69" s="93"/>
+      <c r="AG69" s="93"/>
+      <c r="AH69" s="93"/>
+      <c r="AI69" s="93"/>
+      <c r="AJ69" s="93"/>
+      <c r="AK69" s="93"/>
+      <c r="AL69" s="93"/>
+      <c r="AM69" s="93"/>
+      <c r="AN69" s="93"/>
+      <c r="AO69" s="93"/>
+      <c r="AP69" s="93"/>
+    </row>
+    <row r="70" spans="1:90" ht="22">
       <c r="A70" s="4"/>
       <c r="B70" s="3">
         <v>4</v>
@@ -2755,8 +4933,40 @@
       <c r="J70" s="25">
         <v>342</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" ht="22">
+      <c r="K70" s="93"/>
+      <c r="L70" s="93"/>
+      <c r="M70" s="93"/>
+      <c r="N70" s="93"/>
+      <c r="O70" s="93"/>
+      <c r="P70" s="93"/>
+      <c r="Q70" s="93"/>
+      <c r="R70" s="93"/>
+      <c r="S70" s="93"/>
+      <c r="T70" s="93"/>
+      <c r="U70" s="93"/>
+      <c r="V70" s="93"/>
+      <c r="W70" s="93"/>
+      <c r="X70" s="93"/>
+      <c r="Y70" s="93"/>
+      <c r="Z70" s="93"/>
+      <c r="AA70" s="93"/>
+      <c r="AB70" s="93"/>
+      <c r="AC70" s="93"/>
+      <c r="AD70" s="93"/>
+      <c r="AE70" s="93"/>
+      <c r="AF70" s="93"/>
+      <c r="AG70" s="93"/>
+      <c r="AH70" s="93"/>
+      <c r="AI70" s="93"/>
+      <c r="AJ70" s="93"/>
+      <c r="AK70" s="93"/>
+      <c r="AL70" s="93"/>
+      <c r="AM70" s="93"/>
+      <c r="AN70" s="93"/>
+      <c r="AO70" s="93"/>
+      <c r="AP70" s="93"/>
+    </row>
+    <row r="71" spans="1:90" ht="22">
       <c r="A71" s="4"/>
       <c r="B71" s="3">
         <v>5</v>
@@ -2777,8 +4987,40 @@
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
       <c r="J71" s="12"/>
-    </row>
-    <row r="72" spans="1:10" ht="22">
+      <c r="K71" s="93"/>
+      <c r="L71" s="93"/>
+      <c r="M71" s="93"/>
+      <c r="N71" s="93"/>
+      <c r="O71" s="93"/>
+      <c r="P71" s="93"/>
+      <c r="Q71" s="93"/>
+      <c r="R71" s="93"/>
+      <c r="S71" s="93"/>
+      <c r="T71" s="93"/>
+      <c r="U71" s="93"/>
+      <c r="V71" s="93"/>
+      <c r="W71" s="93"/>
+      <c r="X71" s="93"/>
+      <c r="Y71" s="93"/>
+      <c r="Z71" s="93"/>
+      <c r="AA71" s="93"/>
+      <c r="AB71" s="93"/>
+      <c r="AC71" s="93"/>
+      <c r="AD71" s="93"/>
+      <c r="AE71" s="93"/>
+      <c r="AF71" s="93"/>
+      <c r="AG71" s="93"/>
+      <c r="AH71" s="93"/>
+      <c r="AI71" s="93"/>
+      <c r="AJ71" s="93"/>
+      <c r="AK71" s="93"/>
+      <c r="AL71" s="93"/>
+      <c r="AM71" s="93"/>
+      <c r="AN71" s="93"/>
+      <c r="AO71" s="93"/>
+      <c r="AP71" s="93"/>
+    </row>
+    <row r="72" spans="1:90" ht="22">
       <c r="A72" s="3" t="s">
         <v>12</v>
       </c>
@@ -2797,8 +5039,40 @@
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
       <c r="J72" s="12"/>
-    </row>
-    <row r="73" spans="1:10" ht="22">
+      <c r="K72" s="93"/>
+      <c r="L72" s="93"/>
+      <c r="M72" s="93"/>
+      <c r="N72" s="93"/>
+      <c r="O72" s="93"/>
+      <c r="P72" s="93"/>
+      <c r="Q72" s="93"/>
+      <c r="R72" s="93"/>
+      <c r="S72" s="93"/>
+      <c r="T72" s="93"/>
+      <c r="U72" s="93"/>
+      <c r="V72" s="93"/>
+      <c r="W72" s="93"/>
+      <c r="X72" s="93"/>
+      <c r="Y72" s="93"/>
+      <c r="Z72" s="93"/>
+      <c r="AA72" s="93"/>
+      <c r="AB72" s="93"/>
+      <c r="AC72" s="93"/>
+      <c r="AD72" s="93"/>
+      <c r="AE72" s="93"/>
+      <c r="AF72" s="93"/>
+      <c r="AG72" s="93"/>
+      <c r="AH72" s="93"/>
+      <c r="AI72" s="93"/>
+      <c r="AJ72" s="93"/>
+      <c r="AK72" s="93"/>
+      <c r="AL72" s="93"/>
+      <c r="AM72" s="93"/>
+      <c r="AN72" s="93"/>
+      <c r="AO72" s="93"/>
+      <c r="AP72" s="93"/>
+    </row>
+    <row r="73" spans="1:90" ht="22">
       <c r="A73" s="90" t="s">
         <v>21</v>
       </c>
@@ -2827,7 +5101,7 @@
       <c r="I73" s="64"/>
       <c r="J73" s="65"/>
     </row>
-    <row r="74" spans="1:10" ht="22">
+    <row r="74" spans="1:90" ht="22">
       <c r="A74" s="91"/>
       <c r="B74" s="16" t="s">
         <v>26</v>
@@ -2847,7 +5121,7 @@
       <c r="I74" s="64"/>
       <c r="J74" s="65"/>
     </row>
-    <row r="75" spans="1:10" ht="22" customHeight="1">
+    <row r="75" spans="1:90" ht="22" customHeight="1">
       <c r="A75" s="68"/>
       <c r="B75" s="66" t="s">
         <v>28</v>
@@ -2867,7 +5141,7 @@
       <c r="I75" s="42"/>
       <c r="J75" s="43"/>
     </row>
-    <row r="76" spans="1:10" ht="22" customHeight="1">
+    <row r="76" spans="1:90" ht="22" customHeight="1">
       <c r="A76" s="69"/>
       <c r="B76" s="67"/>
       <c r="C76" s="44"/>
@@ -2879,7 +5153,7 @@
       <c r="I76" s="45"/>
       <c r="J76" s="46"/>
     </row>
-    <row r="77" spans="1:10" s="29" customFormat="1" ht="11">
+    <row r="77" spans="1:90" s="29" customFormat="1" ht="11">
       <c r="A77" s="56"/>
       <c r="B77" s="57"/>
       <c r="C77" s="57"/>
@@ -2891,7 +5165,7 @@
       <c r="I77" s="57"/>
       <c r="J77" s="58"/>
     </row>
-    <row r="78" spans="1:10" ht="22">
+    <row r="78" spans="1:90" ht="22">
       <c r="A78" s="3" t="s">
         <v>3</v>
       </c>
@@ -2919,7 +5193,7 @@
       <c r="I78" s="8"/>
       <c r="J78" s="9"/>
     </row>
-    <row r="79" spans="1:10" ht="22">
+    <row r="79" spans="1:90" ht="22">
       <c r="A79" s="10"/>
       <c r="B79" s="3" t="s">
         <v>8</v>
@@ -2943,7 +5217,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="22">
+    <row r="80" spans="1:90" ht="22">
       <c r="A80" s="4"/>
       <c r="B80" s="3">
         <v>1</v>
@@ -2958,8 +5232,88 @@
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
       <c r="J80" s="12"/>
-    </row>
-    <row r="81" spans="1:10" ht="22">
+      <c r="K80" s="93"/>
+      <c r="L80" s="93"/>
+      <c r="M80" s="93"/>
+      <c r="N80" s="93"/>
+      <c r="O80" s="93"/>
+      <c r="P80" s="93"/>
+      <c r="Q80" s="93"/>
+      <c r="R80" s="93"/>
+      <c r="S80" s="93"/>
+      <c r="T80" s="93"/>
+      <c r="U80" s="93"/>
+      <c r="V80" s="93"/>
+      <c r="W80" s="93"/>
+      <c r="X80" s="93"/>
+      <c r="Y80" s="93"/>
+      <c r="Z80" s="93"/>
+      <c r="AA80" s="93"/>
+      <c r="AB80" s="93"/>
+      <c r="AC80" s="93"/>
+      <c r="AD80" s="93"/>
+      <c r="AE80" s="93"/>
+      <c r="AF80" s="93"/>
+      <c r="AG80" s="93"/>
+      <c r="AH80" s="93"/>
+      <c r="AI80" s="93"/>
+      <c r="AJ80" s="93"/>
+      <c r="AK80" s="93"/>
+      <c r="AL80" s="93"/>
+      <c r="AM80" s="93"/>
+      <c r="AN80" s="93"/>
+      <c r="AO80" s="93"/>
+      <c r="AP80" s="93"/>
+      <c r="AQ80" s="93"/>
+      <c r="AR80" s="93"/>
+      <c r="AS80" s="93"/>
+      <c r="AT80" s="93"/>
+      <c r="AU80" s="93"/>
+      <c r="AV80" s="93"/>
+      <c r="AW80" s="93"/>
+      <c r="AX80" s="93"/>
+      <c r="AY80" s="93"/>
+      <c r="AZ80" s="93"/>
+      <c r="BA80" s="93"/>
+      <c r="BB80" s="93"/>
+      <c r="BC80" s="93"/>
+      <c r="BD80" s="93"/>
+      <c r="BE80" s="93"/>
+      <c r="BF80" s="93"/>
+      <c r="BG80" s="93"/>
+      <c r="BH80" s="93"/>
+      <c r="BI80" s="93"/>
+      <c r="BJ80" s="93"/>
+      <c r="BK80" s="93"/>
+      <c r="BL80" s="93"/>
+      <c r="BM80" s="93"/>
+      <c r="BN80" s="93"/>
+      <c r="BO80" s="93"/>
+      <c r="BP80" s="93"/>
+      <c r="BQ80" s="93"/>
+      <c r="BR80" s="93"/>
+      <c r="BS80" s="93"/>
+      <c r="BT80" s="93"/>
+      <c r="BU80" s="93"/>
+      <c r="BV80" s="93"/>
+      <c r="BW80" s="93"/>
+      <c r="BX80" s="93"/>
+      <c r="BY80" s="93"/>
+      <c r="BZ80" s="93"/>
+      <c r="CA80" s="93"/>
+      <c r="CB80" s="93"/>
+      <c r="CC80" s="93"/>
+      <c r="CD80" s="93"/>
+      <c r="CE80" s="93"/>
+      <c r="CF80" s="93"/>
+      <c r="CG80" s="93"/>
+      <c r="CH80" s="93"/>
+      <c r="CI80" s="93"/>
+      <c r="CJ80" s="93"/>
+      <c r="CK80" s="93"/>
+      <c r="CL80" s="93"/>
+    </row>
+    <row r="81" spans="1:90" ht="22">
       <c r="A81" s="3" t="s">
         <v>10</v>
       </c>
@@ -2982,8 +5336,88 @@
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
       <c r="J81" s="12"/>
-    </row>
-    <row r="82" spans="1:10" ht="22">
+      <c r="K81" s="93"/>
+      <c r="L81" s="93"/>
+      <c r="M81" s="93"/>
+      <c r="N81" s="93"/>
+      <c r="O81" s="93"/>
+      <c r="P81" s="93"/>
+      <c r="Q81" s="93"/>
+      <c r="R81" s="93"/>
+      <c r="S81" s="93"/>
+      <c r="T81" s="93"/>
+      <c r="U81" s="93"/>
+      <c r="V81" s="93"/>
+      <c r="W81" s="93"/>
+      <c r="X81" s="93"/>
+      <c r="Y81" s="93"/>
+      <c r="Z81" s="93"/>
+      <c r="AA81" s="93"/>
+      <c r="AB81" s="93"/>
+      <c r="AC81" s="93"/>
+      <c r="AD81" s="93"/>
+      <c r="AE81" s="93"/>
+      <c r="AF81" s="93"/>
+      <c r="AG81" s="93"/>
+      <c r="AH81" s="93"/>
+      <c r="AI81" s="93"/>
+      <c r="AJ81" s="93"/>
+      <c r="AK81" s="93"/>
+      <c r="AL81" s="93"/>
+      <c r="AM81" s="93"/>
+      <c r="AN81" s="93"/>
+      <c r="AO81" s="93"/>
+      <c r="AP81" s="93"/>
+      <c r="AQ81" s="93"/>
+      <c r="AR81" s="93"/>
+      <c r="AS81" s="93"/>
+      <c r="AT81" s="93"/>
+      <c r="AU81" s="93"/>
+      <c r="AV81" s="93"/>
+      <c r="AW81" s="93"/>
+      <c r="AX81" s="93"/>
+      <c r="AY81" s="93"/>
+      <c r="AZ81" s="93"/>
+      <c r="BA81" s="93"/>
+      <c r="BB81" s="93"/>
+      <c r="BC81" s="93"/>
+      <c r="BD81" s="93"/>
+      <c r="BE81" s="93"/>
+      <c r="BF81" s="93"/>
+      <c r="BG81" s="93"/>
+      <c r="BH81" s="93"/>
+      <c r="BI81" s="93"/>
+      <c r="BJ81" s="93"/>
+      <c r="BK81" s="93"/>
+      <c r="BL81" s="93"/>
+      <c r="BM81" s="93"/>
+      <c r="BN81" s="93"/>
+      <c r="BO81" s="93"/>
+      <c r="BP81" s="93"/>
+      <c r="BQ81" s="93"/>
+      <c r="BR81" s="93"/>
+      <c r="BS81" s="93"/>
+      <c r="BT81" s="93"/>
+      <c r="BU81" s="93"/>
+      <c r="BV81" s="93"/>
+      <c r="BW81" s="93"/>
+      <c r="BX81" s="93"/>
+      <c r="BY81" s="93"/>
+      <c r="BZ81" s="93"/>
+      <c r="CA81" s="93"/>
+      <c r="CB81" s="93"/>
+      <c r="CC81" s="93"/>
+      <c r="CD81" s="93"/>
+      <c r="CE81" s="93"/>
+      <c r="CF81" s="93"/>
+      <c r="CG81" s="93"/>
+      <c r="CH81" s="93"/>
+      <c r="CI81" s="93"/>
+      <c r="CJ81" s="93"/>
+      <c r="CK81" s="93"/>
+      <c r="CL81" s="93"/>
+    </row>
+    <row r="82" spans="1:90" ht="22">
       <c r="A82" s="3" t="s">
         <v>11</v>
       </c>
@@ -3006,8 +5440,88 @@
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
       <c r="J82" s="12"/>
-    </row>
-    <row r="83" spans="1:10" ht="22">
+      <c r="K82" s="93"/>
+      <c r="L82" s="93"/>
+      <c r="M82" s="93"/>
+      <c r="N82" s="93"/>
+      <c r="O82" s="93"/>
+      <c r="P82" s="93"/>
+      <c r="Q82" s="93"/>
+      <c r="R82" s="93"/>
+      <c r="S82" s="93"/>
+      <c r="T82" s="93"/>
+      <c r="U82" s="93"/>
+      <c r="V82" s="93"/>
+      <c r="W82" s="93"/>
+      <c r="X82" s="93"/>
+      <c r="Y82" s="93"/>
+      <c r="Z82" s="93"/>
+      <c r="AA82" s="93"/>
+      <c r="AB82" s="93"/>
+      <c r="AC82" s="93"/>
+      <c r="AD82" s="93"/>
+      <c r="AE82" s="93"/>
+      <c r="AF82" s="93"/>
+      <c r="AG82" s="93"/>
+      <c r="AH82" s="93"/>
+      <c r="AI82" s="93"/>
+      <c r="AJ82" s="93"/>
+      <c r="AK82" s="93"/>
+      <c r="AL82" s="93"/>
+      <c r="AM82" s="93"/>
+      <c r="AN82" s="93"/>
+      <c r="AO82" s="93"/>
+      <c r="AP82" s="93"/>
+      <c r="AQ82" s="93"/>
+      <c r="AR82" s="93"/>
+      <c r="AS82" s="93"/>
+      <c r="AT82" s="93"/>
+      <c r="AU82" s="93"/>
+      <c r="AV82" s="93"/>
+      <c r="AW82" s="93"/>
+      <c r="AX82" s="93"/>
+      <c r="AY82" s="93"/>
+      <c r="AZ82" s="93"/>
+      <c r="BA82" s="93"/>
+      <c r="BB82" s="93"/>
+      <c r="BC82" s="93"/>
+      <c r="BD82" s="93"/>
+      <c r="BE82" s="93"/>
+      <c r="BF82" s="93"/>
+      <c r="BG82" s="93"/>
+      <c r="BH82" s="93"/>
+      <c r="BI82" s="93"/>
+      <c r="BJ82" s="93"/>
+      <c r="BK82" s="93"/>
+      <c r="BL82" s="93"/>
+      <c r="BM82" s="93"/>
+      <c r="BN82" s="93"/>
+      <c r="BO82" s="93"/>
+      <c r="BP82" s="93"/>
+      <c r="BQ82" s="93"/>
+      <c r="BR82" s="93"/>
+      <c r="BS82" s="93"/>
+      <c r="BT82" s="93"/>
+      <c r="BU82" s="93"/>
+      <c r="BV82" s="93"/>
+      <c r="BW82" s="93"/>
+      <c r="BX82" s="93"/>
+      <c r="BY82" s="93"/>
+      <c r="BZ82" s="93"/>
+      <c r="CA82" s="93"/>
+      <c r="CB82" s="93"/>
+      <c r="CC82" s="93"/>
+      <c r="CD82" s="93"/>
+      <c r="CE82" s="93"/>
+      <c r="CF82" s="93"/>
+      <c r="CG82" s="93"/>
+      <c r="CH82" s="93"/>
+      <c r="CI82" s="93"/>
+      <c r="CJ82" s="93"/>
+      <c r="CK82" s="93"/>
+      <c r="CL82" s="93"/>
+    </row>
+    <row r="83" spans="1:90" ht="22">
       <c r="A83" s="4"/>
       <c r="B83" s="3">
         <v>4</v>
@@ -3024,8 +5538,88 @@
       </c>
       <c r="G83" s="23"/>
       <c r="J83" s="12"/>
-    </row>
-    <row r="84" spans="1:10" ht="22">
+      <c r="K83" s="93"/>
+      <c r="L83" s="93"/>
+      <c r="M83" s="93"/>
+      <c r="N83" s="93"/>
+      <c r="O83" s="93"/>
+      <c r="P83" s="93"/>
+      <c r="Q83" s="93"/>
+      <c r="R83" s="93"/>
+      <c r="S83" s="93"/>
+      <c r="T83" s="93"/>
+      <c r="U83" s="93"/>
+      <c r="V83" s="93"/>
+      <c r="W83" s="93"/>
+      <c r="X83" s="93"/>
+      <c r="Y83" s="93"/>
+      <c r="Z83" s="93"/>
+      <c r="AA83" s="93"/>
+      <c r="AB83" s="93"/>
+      <c r="AC83" s="93"/>
+      <c r="AD83" s="93"/>
+      <c r="AE83" s="93"/>
+      <c r="AF83" s="93"/>
+      <c r="AG83" s="93"/>
+      <c r="AH83" s="93"/>
+      <c r="AI83" s="93"/>
+      <c r="AJ83" s="93"/>
+      <c r="AK83" s="93"/>
+      <c r="AL83" s="93"/>
+      <c r="AM83" s="93"/>
+      <c r="AN83" s="93"/>
+      <c r="AO83" s="93"/>
+      <c r="AP83" s="93"/>
+      <c r="AQ83" s="93"/>
+      <c r="AR83" s="93"/>
+      <c r="AS83" s="93"/>
+      <c r="AT83" s="93"/>
+      <c r="AU83" s="93"/>
+      <c r="AV83" s="93"/>
+      <c r="AW83" s="93"/>
+      <c r="AX83" s="93"/>
+      <c r="AY83" s="93"/>
+      <c r="AZ83" s="93"/>
+      <c r="BA83" s="93"/>
+      <c r="BB83" s="93"/>
+      <c r="BC83" s="93"/>
+      <c r="BD83" s="93"/>
+      <c r="BE83" s="93"/>
+      <c r="BF83" s="93"/>
+      <c r="BG83" s="93"/>
+      <c r="BH83" s="93"/>
+      <c r="BI83" s="93"/>
+      <c r="BJ83" s="93"/>
+      <c r="BK83" s="93"/>
+      <c r="BL83" s="93"/>
+      <c r="BM83" s="93"/>
+      <c r="BN83" s="93"/>
+      <c r="BO83" s="93"/>
+      <c r="BP83" s="93"/>
+      <c r="BQ83" s="93"/>
+      <c r="BR83" s="93"/>
+      <c r="BS83" s="93"/>
+      <c r="BT83" s="93"/>
+      <c r="BU83" s="93"/>
+      <c r="BV83" s="93"/>
+      <c r="BW83" s="93"/>
+      <c r="BX83" s="93"/>
+      <c r="BY83" s="93"/>
+      <c r="BZ83" s="93"/>
+      <c r="CA83" s="93"/>
+      <c r="CB83" s="93"/>
+      <c r="CC83" s="93"/>
+      <c r="CD83" s="93"/>
+      <c r="CE83" s="93"/>
+      <c r="CF83" s="93"/>
+      <c r="CG83" s="93"/>
+      <c r="CH83" s="93"/>
+      <c r="CI83" s="93"/>
+      <c r="CJ83" s="93"/>
+      <c r="CK83" s="93"/>
+      <c r="CL83" s="93"/>
+    </row>
+    <row r="84" spans="1:90" ht="22">
       <c r="A84" s="4"/>
       <c r="B84" s="3">
         <v>5</v>
@@ -3042,8 +5636,88 @@
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
       <c r="J84" s="12"/>
-    </row>
-    <row r="85" spans="1:10" ht="22">
+      <c r="K84" s="93"/>
+      <c r="L84" s="93"/>
+      <c r="M84" s="93"/>
+      <c r="N84" s="93"/>
+      <c r="O84" s="93"/>
+      <c r="P84" s="93"/>
+      <c r="Q84" s="93"/>
+      <c r="R84" s="93"/>
+      <c r="S84" s="93"/>
+      <c r="T84" s="93"/>
+      <c r="U84" s="93"/>
+      <c r="V84" s="93"/>
+      <c r="W84" s="93"/>
+      <c r="X84" s="93"/>
+      <c r="Y84" s="93"/>
+      <c r="Z84" s="93"/>
+      <c r="AA84" s="93"/>
+      <c r="AB84" s="93"/>
+      <c r="AC84" s="93"/>
+      <c r="AD84" s="93"/>
+      <c r="AE84" s="93"/>
+      <c r="AF84" s="93"/>
+      <c r="AG84" s="93"/>
+      <c r="AH84" s="93"/>
+      <c r="AI84" s="93"/>
+      <c r="AJ84" s="93"/>
+      <c r="AK84" s="93"/>
+      <c r="AL84" s="93"/>
+      <c r="AM84" s="93"/>
+      <c r="AN84" s="93"/>
+      <c r="AO84" s="93"/>
+      <c r="AP84" s="93"/>
+      <c r="AQ84" s="93"/>
+      <c r="AR84" s="93"/>
+      <c r="AS84" s="93"/>
+      <c r="AT84" s="93"/>
+      <c r="AU84" s="93"/>
+      <c r="AV84" s="93"/>
+      <c r="AW84" s="93"/>
+      <c r="AX84" s="93"/>
+      <c r="AY84" s="93"/>
+      <c r="AZ84" s="93"/>
+      <c r="BA84" s="93"/>
+      <c r="BB84" s="93"/>
+      <c r="BC84" s="93"/>
+      <c r="BD84" s="93"/>
+      <c r="BE84" s="93"/>
+      <c r="BF84" s="93"/>
+      <c r="BG84" s="93"/>
+      <c r="BH84" s="93"/>
+      <c r="BI84" s="93"/>
+      <c r="BJ84" s="93"/>
+      <c r="BK84" s="93"/>
+      <c r="BL84" s="93"/>
+      <c r="BM84" s="93"/>
+      <c r="BN84" s="93"/>
+      <c r="BO84" s="93"/>
+      <c r="BP84" s="93"/>
+      <c r="BQ84" s="93"/>
+      <c r="BR84" s="93"/>
+      <c r="BS84" s="93"/>
+      <c r="BT84" s="93"/>
+      <c r="BU84" s="93"/>
+      <c r="BV84" s="93"/>
+      <c r="BW84" s="93"/>
+      <c r="BX84" s="93"/>
+      <c r="BY84" s="93"/>
+      <c r="BZ84" s="93"/>
+      <c r="CA84" s="93"/>
+      <c r="CB84" s="93"/>
+      <c r="CC84" s="93"/>
+      <c r="CD84" s="93"/>
+      <c r="CE84" s="93"/>
+      <c r="CF84" s="93"/>
+      <c r="CG84" s="93"/>
+      <c r="CH84" s="93"/>
+      <c r="CI84" s="93"/>
+      <c r="CJ84" s="93"/>
+      <c r="CK84" s="93"/>
+      <c r="CL84" s="93"/>
+    </row>
+    <row r="85" spans="1:90" ht="22">
       <c r="A85" s="3" t="s">
         <v>12</v>
       </c>
@@ -3066,8 +5740,88 @@
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
       <c r="J85" s="12"/>
-    </row>
-    <row r="86" spans="1:10" ht="22">
+      <c r="K85" s="93"/>
+      <c r="L85" s="93"/>
+      <c r="M85" s="93"/>
+      <c r="N85" s="93"/>
+      <c r="O85" s="93"/>
+      <c r="P85" s="93"/>
+      <c r="Q85" s="93"/>
+      <c r="R85" s="93"/>
+      <c r="S85" s="93"/>
+      <c r="T85" s="93"/>
+      <c r="U85" s="93"/>
+      <c r="V85" s="93"/>
+      <c r="W85" s="93"/>
+      <c r="X85" s="93"/>
+      <c r="Y85" s="93"/>
+      <c r="Z85" s="93"/>
+      <c r="AA85" s="93"/>
+      <c r="AB85" s="93"/>
+      <c r="AC85" s="93"/>
+      <c r="AD85" s="93"/>
+      <c r="AE85" s="93"/>
+      <c r="AF85" s="93"/>
+      <c r="AG85" s="93"/>
+      <c r="AH85" s="93"/>
+      <c r="AI85" s="93"/>
+      <c r="AJ85" s="93"/>
+      <c r="AK85" s="93"/>
+      <c r="AL85" s="93"/>
+      <c r="AM85" s="93"/>
+      <c r="AN85" s="93"/>
+      <c r="AO85" s="93"/>
+      <c r="AP85" s="93"/>
+      <c r="AQ85" s="93"/>
+      <c r="AR85" s="93"/>
+      <c r="AS85" s="93"/>
+      <c r="AT85" s="93"/>
+      <c r="AU85" s="93"/>
+      <c r="AV85" s="93"/>
+      <c r="AW85" s="93"/>
+      <c r="AX85" s="93"/>
+      <c r="AY85" s="93"/>
+      <c r="AZ85" s="93"/>
+      <c r="BA85" s="93"/>
+      <c r="BB85" s="93"/>
+      <c r="BC85" s="93"/>
+      <c r="BD85" s="93"/>
+      <c r="BE85" s="93"/>
+      <c r="BF85" s="93"/>
+      <c r="BG85" s="93"/>
+      <c r="BH85" s="93"/>
+      <c r="BI85" s="93"/>
+      <c r="BJ85" s="93"/>
+      <c r="BK85" s="93"/>
+      <c r="BL85" s="93"/>
+      <c r="BM85" s="93"/>
+      <c r="BN85" s="93"/>
+      <c r="BO85" s="93"/>
+      <c r="BP85" s="93"/>
+      <c r="BQ85" s="93"/>
+      <c r="BR85" s="93"/>
+      <c r="BS85" s="93"/>
+      <c r="BT85" s="93"/>
+      <c r="BU85" s="93"/>
+      <c r="BV85" s="93"/>
+      <c r="BW85" s="93"/>
+      <c r="BX85" s="93"/>
+      <c r="BY85" s="93"/>
+      <c r="BZ85" s="93"/>
+      <c r="CA85" s="93"/>
+      <c r="CB85" s="93"/>
+      <c r="CC85" s="93"/>
+      <c r="CD85" s="93"/>
+      <c r="CE85" s="93"/>
+      <c r="CF85" s="93"/>
+      <c r="CG85" s="93"/>
+      <c r="CH85" s="93"/>
+      <c r="CI85" s="93"/>
+      <c r="CJ85" s="93"/>
+      <c r="CK85" s="93"/>
+      <c r="CL85" s="93"/>
+    </row>
+    <row r="86" spans="1:90" ht="22">
       <c r="A86" s="85" t="s">
         <v>23</v>
       </c>
@@ -3096,7 +5850,7 @@
       <c r="I86" s="64"/>
       <c r="J86" s="65"/>
     </row>
-    <row r="87" spans="1:10" ht="24">
+    <row r="87" spans="1:90" ht="24">
       <c r="A87" s="86"/>
       <c r="B87" s="16" t="s">
         <v>26</v>
@@ -3116,7 +5870,7 @@
       <c r="I87" s="88"/>
       <c r="J87" s="89"/>
     </row>
-    <row r="88" spans="1:10" ht="22" customHeight="1">
+    <row r="88" spans="1:90" ht="22" customHeight="1">
       <c r="A88" s="74"/>
       <c r="B88" s="26"/>
       <c r="C88" s="50">
@@ -3134,7 +5888,7 @@
       <c r="I88" s="77"/>
       <c r="J88" s="78"/>
     </row>
-    <row r="89" spans="1:10" ht="22" customHeight="1">
+    <row r="89" spans="1:90" ht="22" customHeight="1">
       <c r="A89" s="75"/>
       <c r="B89" s="26"/>
       <c r="C89" s="53"/>
@@ -3146,7 +5900,7 @@
       <c r="I89" s="80"/>
       <c r="J89" s="81"/>
     </row>
-    <row r="90" spans="1:10" s="30" customFormat="1" ht="7">
+    <row r="90" spans="1:90" s="30" customFormat="1" ht="7">
       <c r="A90" s="82"/>
       <c r="B90" s="83"/>
       <c r="C90" s="83"/>
@@ -3158,7 +5912,7 @@
       <c r="I90" s="83"/>
       <c r="J90" s="84"/>
     </row>
-    <row r="91" spans="1:10" ht="22">
+    <row r="91" spans="1:90" ht="22">
       <c r="A91" s="3" t="s">
         <v>3</v>
       </c>
@@ -3186,7 +5940,7 @@
       <c r="I91" s="8"/>
       <c r="J91" s="9"/>
     </row>
-    <row r="92" spans="1:10" ht="22">
+    <row r="92" spans="1:90" ht="22">
       <c r="A92" s="17"/>
       <c r="B92" s="3" t="s">
         <v>8</v>
@@ -3210,7 +5964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="22">
+    <row r="93" spans="1:90" ht="22">
       <c r="A93" s="4"/>
       <c r="B93" s="3">
         <v>1</v>
@@ -3231,8 +5985,69 @@
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
       <c r="J93" s="12"/>
-    </row>
-    <row r="94" spans="1:10" ht="22">
+      <c r="K93" s="93"/>
+      <c r="L93" s="93"/>
+      <c r="M93" s="93"/>
+      <c r="N93" s="93"/>
+      <c r="O93" s="93"/>
+      <c r="P93" s="93"/>
+      <c r="Q93" s="93"/>
+      <c r="R93" s="93"/>
+      <c r="S93" s="93"/>
+      <c r="T93" s="93"/>
+      <c r="U93" s="93"/>
+      <c r="V93" s="93"/>
+      <c r="W93" s="93"/>
+      <c r="X93" s="93"/>
+      <c r="Y93" s="93"/>
+      <c r="Z93" s="93"/>
+      <c r="AA93" s="93"/>
+      <c r="AB93" s="93"/>
+      <c r="AC93" s="93"/>
+      <c r="AD93" s="93"/>
+      <c r="AE93" s="93"/>
+      <c r="AF93" s="93"/>
+      <c r="AG93" s="93"/>
+      <c r="AH93" s="93"/>
+      <c r="AI93" s="93"/>
+      <c r="AJ93" s="93"/>
+      <c r="AK93" s="93"/>
+      <c r="AL93" s="93"/>
+      <c r="AM93" s="93"/>
+      <c r="AN93" s="93"/>
+      <c r="AO93" s="93"/>
+      <c r="AP93" s="93"/>
+      <c r="AQ93" s="93"/>
+      <c r="AR93" s="93"/>
+      <c r="AS93" s="93"/>
+      <c r="AT93" s="93"/>
+      <c r="AU93" s="93"/>
+      <c r="AV93" s="93"/>
+      <c r="AW93" s="93"/>
+      <c r="AX93" s="93"/>
+      <c r="AY93" s="93"/>
+      <c r="AZ93" s="93"/>
+      <c r="BA93" s="93"/>
+      <c r="BB93" s="93"/>
+      <c r="BC93" s="93"/>
+      <c r="BD93" s="93"/>
+      <c r="BE93" s="93"/>
+      <c r="BF93" s="93"/>
+      <c r="BG93" s="93"/>
+      <c r="BH93" s="93"/>
+      <c r="BI93" s="93"/>
+      <c r="BJ93" s="93"/>
+      <c r="BK93" s="93"/>
+      <c r="BL93" s="93"/>
+      <c r="BM93" s="93"/>
+      <c r="BN93" s="93"/>
+      <c r="BO93" s="93"/>
+      <c r="BP93" s="93"/>
+      <c r="BQ93" s="93"/>
+      <c r="BR93" s="93"/>
+      <c r="BS93" s="93"/>
+    </row>
+    <row r="94" spans="1:90" ht="22">
       <c r="A94" s="3" t="s">
         <v>20</v>
       </c>
@@ -3249,8 +6064,69 @@
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
       <c r="J94" s="12"/>
-    </row>
-    <row r="95" spans="1:10" ht="22">
+      <c r="K94" s="93"/>
+      <c r="L94" s="93"/>
+      <c r="M94" s="93"/>
+      <c r="N94" s="93"/>
+      <c r="O94" s="93"/>
+      <c r="P94" s="93"/>
+      <c r="Q94" s="93"/>
+      <c r="R94" s="93"/>
+      <c r="S94" s="93"/>
+      <c r="T94" s="93"/>
+      <c r="U94" s="93"/>
+      <c r="V94" s="93"/>
+      <c r="W94" s="93"/>
+      <c r="X94" s="93"/>
+      <c r="Y94" s="93"/>
+      <c r="Z94" s="93"/>
+      <c r="AA94" s="93"/>
+      <c r="AB94" s="93"/>
+      <c r="AC94" s="93"/>
+      <c r="AD94" s="93"/>
+      <c r="AE94" s="93"/>
+      <c r="AF94" s="93"/>
+      <c r="AG94" s="93"/>
+      <c r="AH94" s="93"/>
+      <c r="AI94" s="93"/>
+      <c r="AJ94" s="93"/>
+      <c r="AK94" s="93"/>
+      <c r="AL94" s="93"/>
+      <c r="AM94" s="93"/>
+      <c r="AN94" s="93"/>
+      <c r="AO94" s="93"/>
+      <c r="AP94" s="93"/>
+      <c r="AQ94" s="93"/>
+      <c r="AR94" s="93"/>
+      <c r="AS94" s="93"/>
+      <c r="AT94" s="93"/>
+      <c r="AU94" s="93"/>
+      <c r="AV94" s="93"/>
+      <c r="AW94" s="93"/>
+      <c r="AX94" s="93"/>
+      <c r="AY94" s="93"/>
+      <c r="AZ94" s="93"/>
+      <c r="BA94" s="93"/>
+      <c r="BB94" s="93"/>
+      <c r="BC94" s="93"/>
+      <c r="BD94" s="93"/>
+      <c r="BE94" s="93"/>
+      <c r="BF94" s="93"/>
+      <c r="BG94" s="93"/>
+      <c r="BH94" s="93"/>
+      <c r="BI94" s="93"/>
+      <c r="BJ94" s="93"/>
+      <c r="BK94" s="93"/>
+      <c r="BL94" s="93"/>
+      <c r="BM94" s="93"/>
+      <c r="BN94" s="93"/>
+      <c r="BO94" s="93"/>
+      <c r="BP94" s="93"/>
+      <c r="BQ94" s="93"/>
+      <c r="BR94" s="93"/>
+      <c r="BS94" s="93"/>
+    </row>
+    <row r="95" spans="1:90" ht="22">
       <c r="A95" s="3" t="s">
         <v>11</v>
       </c>
@@ -3273,8 +6149,69 @@
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
       <c r="J95" s="12"/>
-    </row>
-    <row r="96" spans="1:10" ht="22">
+      <c r="K95" s="93"/>
+      <c r="L95" s="93"/>
+      <c r="M95" s="93"/>
+      <c r="N95" s="93"/>
+      <c r="O95" s="93"/>
+      <c r="P95" s="93"/>
+      <c r="Q95" s="93"/>
+      <c r="R95" s="93"/>
+      <c r="S95" s="93"/>
+      <c r="T95" s="93"/>
+      <c r="U95" s="93"/>
+      <c r="V95" s="93"/>
+      <c r="W95" s="93"/>
+      <c r="X95" s="93"/>
+      <c r="Y95" s="93"/>
+      <c r="Z95" s="93"/>
+      <c r="AA95" s="93"/>
+      <c r="AB95" s="93"/>
+      <c r="AC95" s="93"/>
+      <c r="AD95" s="93"/>
+      <c r="AE95" s="93"/>
+      <c r="AF95" s="93"/>
+      <c r="AG95" s="93"/>
+      <c r="AH95" s="93"/>
+      <c r="AI95" s="93"/>
+      <c r="AJ95" s="93"/>
+      <c r="AK95" s="93"/>
+      <c r="AL95" s="93"/>
+      <c r="AM95" s="93"/>
+      <c r="AN95" s="93"/>
+      <c r="AO95" s="93"/>
+      <c r="AP95" s="93"/>
+      <c r="AQ95" s="93"/>
+      <c r="AR95" s="93"/>
+      <c r="AS95" s="93"/>
+      <c r="AT95" s="93"/>
+      <c r="AU95" s="93"/>
+      <c r="AV95" s="93"/>
+      <c r="AW95" s="93"/>
+      <c r="AX95" s="93"/>
+      <c r="AY95" s="93"/>
+      <c r="AZ95" s="93"/>
+      <c r="BA95" s="93"/>
+      <c r="BB95" s="93"/>
+      <c r="BC95" s="93"/>
+      <c r="BD95" s="93"/>
+      <c r="BE95" s="93"/>
+      <c r="BF95" s="93"/>
+      <c r="BG95" s="93"/>
+      <c r="BH95" s="93"/>
+      <c r="BI95" s="93"/>
+      <c r="BJ95" s="93"/>
+      <c r="BK95" s="93"/>
+      <c r="BL95" s="93"/>
+      <c r="BM95" s="93"/>
+      <c r="BN95" s="93"/>
+      <c r="BO95" s="93"/>
+      <c r="BP95" s="93"/>
+      <c r="BQ95" s="93"/>
+      <c r="BR95" s="93"/>
+      <c r="BS95" s="93"/>
+    </row>
+    <row r="96" spans="1:90" ht="22">
       <c r="A96" s="4"/>
       <c r="B96" s="3">
         <v>4</v>
@@ -3291,8 +6228,69 @@
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
       <c r="J96" s="12"/>
-    </row>
-    <row r="97" spans="1:10" ht="22">
+      <c r="K96" s="93"/>
+      <c r="L96" s="93"/>
+      <c r="M96" s="93"/>
+      <c r="N96" s="93"/>
+      <c r="O96" s="93"/>
+      <c r="P96" s="93"/>
+      <c r="Q96" s="93"/>
+      <c r="R96" s="93"/>
+      <c r="S96" s="93"/>
+      <c r="T96" s="93"/>
+      <c r="U96" s="93"/>
+      <c r="V96" s="93"/>
+      <c r="W96" s="93"/>
+      <c r="X96" s="93"/>
+      <c r="Y96" s="93"/>
+      <c r="Z96" s="93"/>
+      <c r="AA96" s="93"/>
+      <c r="AB96" s="93"/>
+      <c r="AC96" s="93"/>
+      <c r="AD96" s="93"/>
+      <c r="AE96" s="93"/>
+      <c r="AF96" s="93"/>
+      <c r="AG96" s="93"/>
+      <c r="AH96" s="93"/>
+      <c r="AI96" s="93"/>
+      <c r="AJ96" s="93"/>
+      <c r="AK96" s="93"/>
+      <c r="AL96" s="93"/>
+      <c r="AM96" s="93"/>
+      <c r="AN96" s="93"/>
+      <c r="AO96" s="93"/>
+      <c r="AP96" s="93"/>
+      <c r="AQ96" s="93"/>
+      <c r="AR96" s="93"/>
+      <c r="AS96" s="93"/>
+      <c r="AT96" s="93"/>
+      <c r="AU96" s="93"/>
+      <c r="AV96" s="93"/>
+      <c r="AW96" s="93"/>
+      <c r="AX96" s="93"/>
+      <c r="AY96" s="93"/>
+      <c r="AZ96" s="93"/>
+      <c r="BA96" s="93"/>
+      <c r="BB96" s="93"/>
+      <c r="BC96" s="93"/>
+      <c r="BD96" s="93"/>
+      <c r="BE96" s="93"/>
+      <c r="BF96" s="93"/>
+      <c r="BG96" s="93"/>
+      <c r="BH96" s="93"/>
+      <c r="BI96" s="93"/>
+      <c r="BJ96" s="93"/>
+      <c r="BK96" s="93"/>
+      <c r="BL96" s="93"/>
+      <c r="BM96" s="93"/>
+      <c r="BN96" s="93"/>
+      <c r="BO96" s="93"/>
+      <c r="BP96" s="93"/>
+      <c r="BQ96" s="93"/>
+      <c r="BR96" s="93"/>
+      <c r="BS96" s="93"/>
+    </row>
+    <row r="97" spans="1:71" ht="22">
       <c r="A97" s="4"/>
       <c r="B97" s="3">
         <v>5</v>
@@ -3309,8 +6307,69 @@
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
       <c r="J97" s="12"/>
-    </row>
-    <row r="98" spans="1:10" ht="22">
+      <c r="K97" s="93"/>
+      <c r="L97" s="93"/>
+      <c r="M97" s="93"/>
+      <c r="N97" s="93"/>
+      <c r="O97" s="93"/>
+      <c r="P97" s="93"/>
+      <c r="Q97" s="93"/>
+      <c r="R97" s="93"/>
+      <c r="S97" s="93"/>
+      <c r="T97" s="93"/>
+      <c r="U97" s="93"/>
+      <c r="V97" s="93"/>
+      <c r="W97" s="93"/>
+      <c r="X97" s="93"/>
+      <c r="Y97" s="93"/>
+      <c r="Z97" s="93"/>
+      <c r="AA97" s="93"/>
+      <c r="AB97" s="93"/>
+      <c r="AC97" s="93"/>
+      <c r="AD97" s="93"/>
+      <c r="AE97" s="93"/>
+      <c r="AF97" s="93"/>
+      <c r="AG97" s="93"/>
+      <c r="AH97" s="93"/>
+      <c r="AI97" s="93"/>
+      <c r="AJ97" s="93"/>
+      <c r="AK97" s="93"/>
+      <c r="AL97" s="93"/>
+      <c r="AM97" s="93"/>
+      <c r="AN97" s="93"/>
+      <c r="AO97" s="93"/>
+      <c r="AP97" s="93"/>
+      <c r="AQ97" s="93"/>
+      <c r="AR97" s="93"/>
+      <c r="AS97" s="93"/>
+      <c r="AT97" s="93"/>
+      <c r="AU97" s="93"/>
+      <c r="AV97" s="93"/>
+      <c r="AW97" s="93"/>
+      <c r="AX97" s="93"/>
+      <c r="AY97" s="93"/>
+      <c r="AZ97" s="93"/>
+      <c r="BA97" s="93"/>
+      <c r="BB97" s="93"/>
+      <c r="BC97" s="93"/>
+      <c r="BD97" s="93"/>
+      <c r="BE97" s="93"/>
+      <c r="BF97" s="93"/>
+      <c r="BG97" s="93"/>
+      <c r="BH97" s="93"/>
+      <c r="BI97" s="93"/>
+      <c r="BJ97" s="93"/>
+      <c r="BK97" s="93"/>
+      <c r="BL97" s="93"/>
+      <c r="BM97" s="93"/>
+      <c r="BN97" s="93"/>
+      <c r="BO97" s="93"/>
+      <c r="BP97" s="93"/>
+      <c r="BQ97" s="93"/>
+      <c r="BR97" s="93"/>
+      <c r="BS97" s="93"/>
+    </row>
+    <row r="98" spans="1:71" ht="22">
       <c r="A98" s="3" t="s">
         <v>12</v>
       </c>
@@ -3333,8 +6392,69 @@
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
       <c r="J98" s="12"/>
-    </row>
-    <row r="99" spans="1:10" ht="22">
+      <c r="K98" s="93"/>
+      <c r="L98" s="93"/>
+      <c r="M98" s="93"/>
+      <c r="N98" s="93"/>
+      <c r="O98" s="93"/>
+      <c r="P98" s="93"/>
+      <c r="Q98" s="93"/>
+      <c r="R98" s="93"/>
+      <c r="S98" s="93"/>
+      <c r="T98" s="93"/>
+      <c r="U98" s="93"/>
+      <c r="V98" s="93"/>
+      <c r="W98" s="93"/>
+      <c r="X98" s="93"/>
+      <c r="Y98" s="93"/>
+      <c r="Z98" s="93"/>
+      <c r="AA98" s="93"/>
+      <c r="AB98" s="93"/>
+      <c r="AC98" s="93"/>
+      <c r="AD98" s="93"/>
+      <c r="AE98" s="93"/>
+      <c r="AF98" s="93"/>
+      <c r="AG98" s="93"/>
+      <c r="AH98" s="93"/>
+      <c r="AI98" s="93"/>
+      <c r="AJ98" s="93"/>
+      <c r="AK98" s="93"/>
+      <c r="AL98" s="93"/>
+      <c r="AM98" s="93"/>
+      <c r="AN98" s="93"/>
+      <c r="AO98" s="93"/>
+      <c r="AP98" s="93"/>
+      <c r="AQ98" s="93"/>
+      <c r="AR98" s="93"/>
+      <c r="AS98" s="93"/>
+      <c r="AT98" s="93"/>
+      <c r="AU98" s="93"/>
+      <c r="AV98" s="93"/>
+      <c r="AW98" s="93"/>
+      <c r="AX98" s="93"/>
+      <c r="AY98" s="93"/>
+      <c r="AZ98" s="93"/>
+      <c r="BA98" s="93"/>
+      <c r="BB98" s="93"/>
+      <c r="BC98" s="93"/>
+      <c r="BD98" s="93"/>
+      <c r="BE98" s="93"/>
+      <c r="BF98" s="93"/>
+      <c r="BG98" s="93"/>
+      <c r="BH98" s="93"/>
+      <c r="BI98" s="93"/>
+      <c r="BJ98" s="93"/>
+      <c r="BK98" s="93"/>
+      <c r="BL98" s="93"/>
+      <c r="BM98" s="93"/>
+      <c r="BN98" s="93"/>
+      <c r="BO98" s="93"/>
+      <c r="BP98" s="93"/>
+      <c r="BQ98" s="93"/>
+      <c r="BR98" s="93"/>
+      <c r="BS98" s="93"/>
+    </row>
+    <row r="99" spans="1:71" ht="22">
       <c r="A99" s="85" t="s">
         <v>24</v>
       </c>
@@ -3361,7 +6481,7 @@
       <c r="I99" s="64"/>
       <c r="J99" s="65"/>
     </row>
-    <row r="100" spans="1:10" ht="22">
+    <row r="100" spans="1:71" ht="22">
       <c r="A100" s="86"/>
       <c r="B100" s="16" t="s">
         <v>26</v>
@@ -3381,7 +6501,7 @@
       <c r="I100" s="64"/>
       <c r="J100" s="65"/>
     </row>
-    <row r="101" spans="1:10" ht="22" customHeight="1">
+    <row r="101" spans="1:71" ht="22" customHeight="1">
       <c r="A101" s="68"/>
       <c r="B101" s="66" t="s">
         <v>28</v>
@@ -3401,7 +6521,7 @@
       <c r="I101" s="42"/>
       <c r="J101" s="43"/>
     </row>
-    <row r="102" spans="1:10" ht="22" customHeight="1">
+    <row r="102" spans="1:71" ht="22" customHeight="1">
       <c r="A102" s="69"/>
       <c r="B102" s="67"/>
       <c r="C102" s="44"/>
@@ -3413,7 +6533,7 @@
       <c r="I102" s="45"/>
       <c r="J102" s="46"/>
     </row>
-    <row r="103" spans="1:10" ht="22" customHeight="1">
+    <row r="103" spans="1:71" ht="22" customHeight="1">
       <c r="A103" s="31"/>
       <c r="B103" s="32"/>
       <c r="C103" s="27"/>
@@ -3425,7 +6545,7 @@
       <c r="I103" s="33"/>
       <c r="J103" s="33"/>
     </row>
-    <row r="104" spans="1:10" s="37" customFormat="1" ht="32">
+    <row r="104" spans="1:71" s="37" customFormat="1" ht="32">
       <c r="A104" s="70" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
not sure if last one went in
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/speedy/Documents/GitProjects/AmpSheetRepository/AmpSheetMain/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DA42B6-F7AF-9F4A-94EE-BBF0135AB3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4322191E-855B-134D-B418-BDACED3D723D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20520" xr2:uid="{329AA3C5-52D5-8A41-A20D-B75AE869BCAA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20380" xr2:uid="{329AA3C5-52D5-8A41-A20D-B75AE869BCAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Racks" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="32">
   <si>
     <t>ChanLow</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1103,8 +1106,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:DU104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K93" sqref="K93:BS98"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L93" sqref="K93:BS98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5985,7 +5988,9 @@
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
       <c r="J93" s="12"/>
-      <c r="K93" s="93"/>
+      <c r="K93" s="93" t="s">
+        <v>31</v>
+      </c>
       <c r="L93" s="93"/>
       <c r="M93" s="93"/>
       <c r="N93" s="93"/>

</xml_diff>

<commit_message>
just getting the right way to get the list
not there yet
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/speedy/Documents/GitProjects/AmpSheetRepository/AmpSheetMain/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C10380B-C9BE-9A4F-A38F-ED50F1710D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081CC1FD-BEF7-4941-B6CB-37FE7D3C791F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="760" windowWidth="34560" windowHeight="20380" xr2:uid="{329AA3C5-52D5-8A41-A20D-B75AE869BCAA}"/>
   </bookViews>
@@ -1101,8 +1101,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:DU104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J98" sqref="J98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
couple things in test2 changed
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/speedy/Documents/GitProjects/AmpSheetRepository/AmpSheetMain/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AC128C-A38E-CB4E-8C8E-398FE23AEA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB05480-9055-4A44-8B97-16C2900CACB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" xr2:uid="{329AA3C5-52D5-8A41-A20D-B75AE869BCAA}"/>
+    <workbookView xWindow="840" yWindow="-20360" windowWidth="34560" windowHeight="20360" xr2:uid="{329AA3C5-52D5-8A41-A20D-B75AE869BCAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Racks" sheetId="1" r:id="rId1"/>
     <sheet name="Watts" sheetId="2" r:id="rId2"/>
-    <sheet name="Tab3" sheetId="3" r:id="rId3"/>
+    <sheet name="Dict" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Racks!$A$1:$J$102</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="47">
   <si>
     <t>ChanLow</t>
   </si>
@@ -118,9 +118,6 @@
     <t>M13</t>
   </si>
   <si>
-    <t>48 way rack</t>
-  </si>
-  <si>
     <t>Totals</t>
   </si>
   <si>
@@ -134,6 +131,57 @@
   </si>
   <si>
     <t>Voltage</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>amp1</t>
+  </si>
+  <si>
+    <t>amp2</t>
+  </si>
+  <si>
+    <t>totWatts</t>
+  </si>
+  <si>
+    <t>I104</t>
+  </si>
+  <si>
+    <t>Total Rack Watts =</t>
   </si>
 </sst>
 </file>
@@ -590,6 +638,88 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -620,55 +750,22 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -678,40 +775,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -722,42 +789,23 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1096,8 +1144,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:DU104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K104" sqref="K104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1139,9 +1187,9 @@
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
       <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2017,11 +2065,11 @@
       <c r="DU8" s="37"/>
     </row>
     <row r="9" spans="1:125" ht="22">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="61" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="12">
         <f>SUM(C3:C8)</f>
@@ -2038,12 +2086,12 @@
       <c r="F9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="62" t="s">
+      <c r="G9" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="64"/>
       <c r="K9" s="40"/>
       <c r="L9" s="40"/>
       <c r="M9" s="40"/>
@@ -2056,24 +2104,24 @@
       <c r="T9" s="46"/>
     </row>
     <row r="10" spans="1:125" ht="24">
-      <c r="A10" s="61"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="93">
+        <v>25</v>
+      </c>
+      <c r="C10" s="56">
         <f>SUM(C9:E9)</f>
         <v>52.339999999999996</v>
       </c>
-      <c r="D10" s="94"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="95"/>
-      <c r="G10" s="91">
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="65">
         <f>ROUNDUP(SUM(C9:E9)/3,2)</f>
         <v>17.450000000000003</v>
       </c>
-      <c r="H10" s="92"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
       <c r="K10" s="40"/>
       <c r="L10" s="40"/>
       <c r="M10" s="40"/>
@@ -2086,22 +2134,22 @@
       <c r="T10" s="46"/>
     </row>
     <row r="11" spans="1:125" ht="22" customHeight="1">
-      <c r="A11" s="66"/>
+      <c r="A11" s="67"/>
       <c r="B11" s="15"/>
-      <c r="C11" s="50">
+      <c r="C11" s="73">
         <f>C10</f>
         <v>52.339999999999996</v>
       </c>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="68">
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="69">
         <f>G10</f>
         <v>17.450000000000003</v>
       </c>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="70"/>
       <c r="K11" s="40"/>
       <c r="L11" s="40"/>
       <c r="M11" s="40"/>
@@ -2114,16 +2162,16 @@
       <c r="T11" s="46"/>
     </row>
     <row r="12" spans="1:125" ht="22" customHeight="1">
-      <c r="A12" s="67"/>
+      <c r="A12" s="68"/>
       <c r="B12" s="15"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="72"/>
       <c r="K12" s="40"/>
       <c r="L12" s="40"/>
       <c r="M12" s="40"/>
@@ -2136,16 +2184,16 @@
       <c r="T12" s="46"/>
     </row>
     <row r="13" spans="1:125" s="27" customFormat="1" ht="11">
-      <c r="A13" s="56"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
+      <c r="A13" s="79"/>
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="80"/>
+      <c r="I13" s="80"/>
+      <c r="J13" s="80"/>
       <c r="K13" s="42"/>
       <c r="L13" s="42"/>
       <c r="M13" s="42"/>
@@ -2200,9 +2248,9 @@
       <c r="B15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
       <c r="F15" s="3" t="s">
         <v>9</v>
       </c>
@@ -2658,11 +2706,11 @@
       <c r="BE21" s="37"/>
     </row>
     <row r="22" spans="1:121" ht="22">
-      <c r="A22" s="60" t="s">
+      <c r="A22" s="61" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="17">
         <f>SUM(C16:C21)</f>
@@ -2679,12 +2727,12 @@
       <c r="F22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="62" t="s">
+      <c r="G22" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="63"/>
-      <c r="I22" s="63"/>
-      <c r="J22" s="63"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="64"/>
       <c r="K22" s="40"/>
       <c r="L22" s="40"/>
       <c r="M22" s="40"/>
@@ -2697,24 +2745,24 @@
       <c r="T22" s="46"/>
     </row>
     <row r="23" spans="1:121" ht="22">
-      <c r="A23" s="61"/>
+      <c r="A23" s="62"/>
       <c r="B23" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="88">
+        <v>25</v>
+      </c>
+      <c r="C23" s="83">
         <f>SUM(C22:E22)</f>
         <v>41.06</v>
       </c>
-      <c r="D23" s="89"/>
-      <c r="E23" s="89"/>
-      <c r="F23" s="90"/>
-      <c r="G23" s="62">
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="63">
         <f>ROUNDUP(SUM(C22:E22)/3,2)</f>
         <v>13.69</v>
       </c>
-      <c r="H23" s="63"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="63"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="64"/>
       <c r="K23" s="40"/>
       <c r="L23" s="40"/>
       <c r="M23" s="40"/>
@@ -2727,24 +2775,24 @@
       <c r="T23" s="46"/>
     </row>
     <row r="24" spans="1:121" ht="22" customHeight="1">
-      <c r="A24" s="72"/>
-      <c r="B24" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="74">
+      <c r="A24" s="86"/>
+      <c r="B24" s="88" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="50">
         <f>SUM(C11+C23)</f>
         <v>93.4</v>
       </c>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="82"/>
-      <c r="G24" s="74">
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="50">
         <f>SUM(G11+G23)</f>
         <v>31.14</v>
       </c>
-      <c r="H24" s="75"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="75"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
       <c r="K24" s="40"/>
       <c r="L24" s="40"/>
       <c r="M24" s="40"/>
@@ -2757,16 +2805,16 @@
       <c r="T24" s="46"/>
     </row>
     <row r="25" spans="1:121" ht="22" customHeight="1">
-      <c r="A25" s="73"/>
-      <c r="B25" s="65"/>
-      <c r="C25" s="76"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="76"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77"/>
-      <c r="J25" s="77"/>
+      <c r="A25" s="87"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
       <c r="K25" s="40"/>
       <c r="L25" s="40"/>
       <c r="M25" s="40"/>
@@ -2821,9 +2869,9 @@
       <c r="B27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="58"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
       <c r="F27" s="3" t="s">
         <v>9</v>
       </c>
@@ -3665,11 +3713,11 @@
       <c r="DQ33" s="37"/>
     </row>
     <row r="34" spans="1:121" ht="22">
-      <c r="A34" s="60" t="s">
+      <c r="A34" s="61" t="s">
         <v>17</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C34" s="12">
         <f>SUM(C28:C33)</f>
@@ -3686,12 +3734,12 @@
       <c r="F34" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G34" s="62" t="s">
+      <c r="G34" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="H34" s="63"/>
-      <c r="I34" s="63"/>
-      <c r="J34" s="63"/>
+      <c r="H34" s="64"/>
+      <c r="I34" s="64"/>
+      <c r="J34" s="64"/>
       <c r="K34" s="40"/>
       <c r="L34" s="40"/>
       <c r="M34" s="40"/>
@@ -3704,24 +3752,24 @@
       <c r="T34" s="46"/>
     </row>
     <row r="35" spans="1:121" ht="24">
-      <c r="A35" s="61"/>
+      <c r="A35" s="62"/>
       <c r="B35" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="93">
+        <v>25</v>
+      </c>
+      <c r="C35" s="56">
         <f>SUM(C34:E34)</f>
         <v>44.12</v>
       </c>
-      <c r="D35" s="94"/>
-      <c r="E35" s="94"/>
-      <c r="F35" s="95"/>
-      <c r="G35" s="91">
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="65">
         <f>ROUNDUP(SUM(C34:E34)/3,2)</f>
         <v>14.709999999999999</v>
       </c>
-      <c r="H35" s="92"/>
-      <c r="I35" s="92"/>
-      <c r="J35" s="92"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="66"/>
+      <c r="J35" s="66"/>
       <c r="K35" s="40"/>
       <c r="L35" s="40"/>
       <c r="M35" s="40"/>
@@ -3734,22 +3782,22 @@
       <c r="T35" s="46"/>
     </row>
     <row r="36" spans="1:121" ht="22" customHeight="1">
-      <c r="A36" s="66"/>
+      <c r="A36" s="67"/>
       <c r="B36" s="15"/>
-      <c r="C36" s="50">
+      <c r="C36" s="73">
         <f>C35</f>
         <v>44.12</v>
       </c>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="68">
+      <c r="D36" s="74"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="69">
         <f>G35</f>
         <v>14.709999999999999</v>
       </c>
-      <c r="H36" s="69"/>
-      <c r="I36" s="69"/>
-      <c r="J36" s="69"/>
+      <c r="H36" s="70"/>
+      <c r="I36" s="70"/>
+      <c r="J36" s="70"/>
       <c r="K36" s="40"/>
       <c r="L36" s="40"/>
       <c r="M36" s="40"/>
@@ -3762,16 +3810,16 @@
       <c r="T36" s="46"/>
     </row>
     <row r="37" spans="1:121" ht="22" customHeight="1">
-      <c r="A37" s="67"/>
+      <c r="A37" s="68"/>
       <c r="B37" s="15"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="71"/>
-      <c r="I37" s="71"/>
-      <c r="J37" s="71"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="78"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="72"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="72"/>
       <c r="K37" s="40"/>
       <c r="L37" s="40"/>
       <c r="M37" s="40"/>
@@ -3784,16 +3832,16 @@
       <c r="T37" s="46"/>
     </row>
     <row r="38" spans="1:121" s="27" customFormat="1" ht="11">
-      <c r="A38" s="56"/>
-      <c r="B38" s="57"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="57"/>
-      <c r="E38" s="57"/>
-      <c r="F38" s="57"/>
-      <c r="G38" s="57"/>
-      <c r="H38" s="57"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="57"/>
+      <c r="A38" s="79"/>
+      <c r="B38" s="80"/>
+      <c r="C38" s="80"/>
+      <c r="D38" s="80"/>
+      <c r="E38" s="80"/>
+      <c r="F38" s="80"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="80"/>
+      <c r="I38" s="80"/>
+      <c r="J38" s="80"/>
       <c r="K38" s="42"/>
       <c r="L38" s="42"/>
       <c r="M38" s="42"/>
@@ -3848,9 +3896,9 @@
       <c r="B40" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="58"/>
-      <c r="D40" s="59"/>
-      <c r="E40" s="59"/>
+      <c r="C40" s="59"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="60"/>
       <c r="F40" s="3" t="s">
         <v>9</v>
       </c>
@@ -4269,11 +4317,11 @@
       <c r="AW46" s="37"/>
     </row>
     <row r="47" spans="1:121" ht="22">
-      <c r="A47" s="96" t="s">
+      <c r="A47" s="81" t="s">
         <v>18</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C47" s="17">
         <f>SUM(C41:C46)</f>
@@ -4290,12 +4338,12 @@
       <c r="F47" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G47" s="62" t="s">
+      <c r="G47" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="H47" s="63"/>
-      <c r="I47" s="63"/>
-      <c r="J47" s="63"/>
+      <c r="H47" s="64"/>
+      <c r="I47" s="64"/>
+      <c r="J47" s="64"/>
       <c r="K47" s="40"/>
       <c r="L47" s="40"/>
       <c r="M47" s="40"/>
@@ -4308,24 +4356,24 @@
       <c r="T47" s="46"/>
     </row>
     <row r="48" spans="1:121" ht="22">
-      <c r="A48" s="97"/>
+      <c r="A48" s="82"/>
       <c r="B48" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C48" s="88">
+        <v>25</v>
+      </c>
+      <c r="C48" s="83">
         <f>SUM(C47:E47)</f>
         <v>48.680000000000007</v>
       </c>
-      <c r="D48" s="89"/>
-      <c r="E48" s="89"/>
-      <c r="F48" s="90"/>
-      <c r="G48" s="62">
+      <c r="D48" s="84"/>
+      <c r="E48" s="84"/>
+      <c r="F48" s="85"/>
+      <c r="G48" s="63">
         <f>ROUNDUP(SUM(C47:E47)/3,2)</f>
         <v>16.23</v>
       </c>
-      <c r="H48" s="63"/>
-      <c r="I48" s="63"/>
-      <c r="J48" s="63"/>
+      <c r="H48" s="64"/>
+      <c r="I48" s="64"/>
+      <c r="J48" s="64"/>
       <c r="K48" s="40"/>
       <c r="L48" s="40"/>
       <c r="M48" s="40"/>
@@ -4338,24 +4386,24 @@
       <c r="T48" s="46"/>
     </row>
     <row r="49" spans="1:47" ht="22" customHeight="1">
-      <c r="A49" s="72"/>
-      <c r="B49" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="C49" s="74">
+      <c r="A49" s="86"/>
+      <c r="B49" s="88" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="50">
         <f>SUM(C36+C48)</f>
         <v>92.800000000000011</v>
       </c>
-      <c r="D49" s="75"/>
-      <c r="E49" s="75"/>
-      <c r="F49" s="82"/>
-      <c r="G49" s="74">
+      <c r="D49" s="51"/>
+      <c r="E49" s="51"/>
+      <c r="F49" s="52"/>
+      <c r="G49" s="50">
         <f>SUM(G36+G48)</f>
         <v>30.939999999999998</v>
       </c>
-      <c r="H49" s="75"/>
-      <c r="I49" s="75"/>
-      <c r="J49" s="75"/>
+      <c r="H49" s="51"/>
+      <c r="I49" s="51"/>
+      <c r="J49" s="51"/>
       <c r="K49" s="40"/>
       <c r="L49" s="40"/>
       <c r="M49" s="40"/>
@@ -4368,16 +4416,16 @@
       <c r="T49" s="46"/>
     </row>
     <row r="50" spans="1:47" ht="22" customHeight="1">
-      <c r="A50" s="73"/>
-      <c r="B50" s="65"/>
-      <c r="C50" s="76"/>
-      <c r="D50" s="77"/>
-      <c r="E50" s="77"/>
-      <c r="F50" s="83"/>
-      <c r="G50" s="76"/>
-      <c r="H50" s="77"/>
-      <c r="I50" s="77"/>
-      <c r="J50" s="77"/>
+      <c r="A50" s="87"/>
+      <c r="B50" s="89"/>
+      <c r="C50" s="53"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="55"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="54"/>
+      <c r="I50" s="54"/>
+      <c r="J50" s="54"/>
       <c r="K50" s="40"/>
       <c r="L50" s="40"/>
       <c r="M50" s="40"/>
@@ -4390,16 +4438,16 @@
       <c r="T50" s="46"/>
     </row>
     <row r="51" spans="1:47" s="27" customFormat="1" ht="11">
-      <c r="A51" s="56"/>
-      <c r="B51" s="57"/>
-      <c r="C51" s="57"/>
-      <c r="D51" s="57"/>
-      <c r="E51" s="57"/>
-      <c r="F51" s="57"/>
-      <c r="G51" s="57"/>
-      <c r="H51" s="57"/>
-      <c r="I51" s="57"/>
-      <c r="J51" s="57"/>
+      <c r="A51" s="79"/>
+      <c r="B51" s="80"/>
+      <c r="C51" s="80"/>
+      <c r="D51" s="80"/>
+      <c r="E51" s="80"/>
+      <c r="F51" s="80"/>
+      <c r="G51" s="80"/>
+      <c r="H51" s="80"/>
+      <c r="I51" s="80"/>
+      <c r="J51" s="80"/>
       <c r="K51" s="42"/>
       <c r="L51" s="42"/>
       <c r="M51" s="42"/>
@@ -4454,9 +4502,9 @@
       <c r="B53" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="58"/>
-      <c r="D53" s="59"/>
-      <c r="E53" s="59"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="60"/>
+      <c r="E53" s="60"/>
       <c r="F53" s="3" t="s">
         <v>9</v>
       </c>
@@ -4852,11 +4900,11 @@
       <c r="AU59" s="37"/>
     </row>
     <row r="60" spans="1:47" ht="22">
-      <c r="A60" s="96" t="s">
+      <c r="A60" s="81" t="s">
         <v>19</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C60" s="12">
         <f>SUM(C54:C59)</f>
@@ -4873,12 +4921,12 @@
       <c r="F60" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G60" s="62" t="s">
+      <c r="G60" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="H60" s="63"/>
-      <c r="I60" s="63"/>
-      <c r="J60" s="63"/>
+      <c r="H60" s="64"/>
+      <c r="I60" s="64"/>
+      <c r="J60" s="64"/>
       <c r="K60" s="40"/>
       <c r="L60" s="40"/>
       <c r="M60" s="40"/>
@@ -4891,24 +4939,24 @@
       <c r="T60" s="46"/>
     </row>
     <row r="61" spans="1:47" ht="24">
-      <c r="A61" s="97"/>
+      <c r="A61" s="82"/>
       <c r="B61" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C61" s="93">
+        <v>25</v>
+      </c>
+      <c r="C61" s="56">
         <f>SUM(C60:E60)</f>
         <v>41.06</v>
       </c>
-      <c r="D61" s="94"/>
-      <c r="E61" s="94"/>
-      <c r="F61" s="95"/>
-      <c r="G61" s="91">
+      <c r="D61" s="57"/>
+      <c r="E61" s="57"/>
+      <c r="F61" s="58"/>
+      <c r="G61" s="65">
         <f>ROUNDUP(SUM(C60:E60)/3,2)</f>
         <v>13.69</v>
       </c>
-      <c r="H61" s="92"/>
-      <c r="I61" s="92"/>
-      <c r="J61" s="92"/>
+      <c r="H61" s="66"/>
+      <c r="I61" s="66"/>
+      <c r="J61" s="66"/>
       <c r="K61" s="40"/>
       <c r="L61" s="40"/>
       <c r="M61" s="40"/>
@@ -4921,22 +4969,22 @@
       <c r="T61" s="46"/>
     </row>
     <row r="62" spans="1:47" ht="22" customHeight="1">
-      <c r="A62" s="66"/>
+      <c r="A62" s="67"/>
       <c r="B62" s="15"/>
-      <c r="C62" s="50">
+      <c r="C62" s="73">
         <f>C61</f>
         <v>41.06</v>
       </c>
-      <c r="D62" s="51"/>
-      <c r="E62" s="51"/>
-      <c r="F62" s="52"/>
-      <c r="G62" s="68">
+      <c r="D62" s="74"/>
+      <c r="E62" s="74"/>
+      <c r="F62" s="75"/>
+      <c r="G62" s="69">
         <f>G61</f>
         <v>13.69</v>
       </c>
-      <c r="H62" s="69"/>
-      <c r="I62" s="69"/>
-      <c r="J62" s="69"/>
+      <c r="H62" s="70"/>
+      <c r="I62" s="70"/>
+      <c r="J62" s="70"/>
       <c r="K62" s="40"/>
       <c r="L62" s="40"/>
       <c r="M62" s="40"/>
@@ -4949,16 +4997,16 @@
       <c r="T62" s="46"/>
     </row>
     <row r="63" spans="1:47" ht="22" customHeight="1">
-      <c r="A63" s="67"/>
+      <c r="A63" s="68"/>
       <c r="B63" s="15"/>
-      <c r="C63" s="53"/>
-      <c r="D63" s="54"/>
-      <c r="E63" s="54"/>
-      <c r="F63" s="55"/>
-      <c r="G63" s="70"/>
-      <c r="H63" s="71"/>
-      <c r="I63" s="71"/>
-      <c r="J63" s="71"/>
+      <c r="C63" s="76"/>
+      <c r="D63" s="77"/>
+      <c r="E63" s="77"/>
+      <c r="F63" s="78"/>
+      <c r="G63" s="71"/>
+      <c r="H63" s="72"/>
+      <c r="I63" s="72"/>
+      <c r="J63" s="72"/>
       <c r="K63" s="40"/>
       <c r="L63" s="40"/>
       <c r="M63" s="40"/>
@@ -4971,16 +5019,16 @@
       <c r="T63" s="46"/>
     </row>
     <row r="64" spans="1:47" s="27" customFormat="1" ht="11">
-      <c r="A64" s="56"/>
-      <c r="B64" s="57"/>
-      <c r="C64" s="57"/>
-      <c r="D64" s="57"/>
-      <c r="E64" s="57"/>
-      <c r="F64" s="57"/>
-      <c r="G64" s="57"/>
-      <c r="H64" s="57"/>
-      <c r="I64" s="57"/>
-      <c r="J64" s="57"/>
+      <c r="A64" s="79"/>
+      <c r="B64" s="80"/>
+      <c r="C64" s="80"/>
+      <c r="D64" s="80"/>
+      <c r="E64" s="80"/>
+      <c r="F64" s="80"/>
+      <c r="G64" s="80"/>
+      <c r="H64" s="80"/>
+      <c r="I64" s="80"/>
+      <c r="J64" s="80"/>
       <c r="K64" s="42"/>
       <c r="L64" s="42"/>
       <c r="M64" s="42"/>
@@ -5035,9 +5083,9 @@
       <c r="B66" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C66" s="58"/>
-      <c r="D66" s="59"/>
-      <c r="E66" s="59"/>
+      <c r="C66" s="59"/>
+      <c r="D66" s="60"/>
+      <c r="E66" s="60"/>
       <c r="F66" s="3" t="s">
         <v>9</v>
       </c>
@@ -5405,11 +5453,11 @@
       <c r="AP72" s="37"/>
     </row>
     <row r="73" spans="1:90" ht="22">
-      <c r="A73" s="96" t="s">
+      <c r="A73" s="81" t="s">
         <v>21</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C73" s="17">
         <f>SUM(C67:C72)</f>
@@ -5426,12 +5474,12 @@
       <c r="F73" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G73" s="62" t="s">
+      <c r="G73" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="H73" s="63"/>
-      <c r="I73" s="63"/>
-      <c r="J73" s="63"/>
+      <c r="H73" s="64"/>
+      <c r="I73" s="64"/>
+      <c r="J73" s="64"/>
       <c r="K73" s="40"/>
       <c r="L73" s="40"/>
       <c r="M73" s="40"/>
@@ -5444,24 +5492,24 @@
       <c r="T73" s="46"/>
     </row>
     <row r="74" spans="1:90" ht="22">
-      <c r="A74" s="97"/>
+      <c r="A74" s="82"/>
       <c r="B74" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C74" s="88">
+        <v>25</v>
+      </c>
+      <c r="C74" s="83">
         <f>SUM(C73:E73)</f>
         <v>44.14</v>
       </c>
-      <c r="D74" s="89"/>
-      <c r="E74" s="89"/>
-      <c r="F74" s="90"/>
-      <c r="G74" s="62">
+      <c r="D74" s="84"/>
+      <c r="E74" s="84"/>
+      <c r="F74" s="85"/>
+      <c r="G74" s="63">
         <f>ROUNDUP(SUM(C73:E73)/3,2)</f>
         <v>14.72</v>
       </c>
-      <c r="H74" s="63"/>
-      <c r="I74" s="63"/>
-      <c r="J74" s="63"/>
+      <c r="H74" s="64"/>
+      <c r="I74" s="64"/>
+      <c r="J74" s="64"/>
       <c r="K74" s="40"/>
       <c r="L74" s="40"/>
       <c r="M74" s="40"/>
@@ -5474,24 +5522,24 @@
       <c r="T74" s="46"/>
     </row>
     <row r="75" spans="1:90" ht="22" customHeight="1">
-      <c r="A75" s="72"/>
-      <c r="B75" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="C75" s="74">
+      <c r="A75" s="86"/>
+      <c r="B75" s="88" t="s">
+        <v>27</v>
+      </c>
+      <c r="C75" s="50">
         <f>SUM(C62+C74)</f>
         <v>85.2</v>
       </c>
-      <c r="D75" s="75"/>
-      <c r="E75" s="75"/>
-      <c r="F75" s="82"/>
-      <c r="G75" s="74">
+      <c r="D75" s="51"/>
+      <c r="E75" s="51"/>
+      <c r="F75" s="52"/>
+      <c r="G75" s="50">
         <f>SUM(G62+G74)</f>
         <v>28.41</v>
       </c>
-      <c r="H75" s="75"/>
-      <c r="I75" s="75"/>
-      <c r="J75" s="75"/>
+      <c r="H75" s="51"/>
+      <c r="I75" s="51"/>
+      <c r="J75" s="51"/>
       <c r="K75" s="40"/>
       <c r="L75" s="40"/>
       <c r="M75" s="40"/>
@@ -5504,16 +5552,16 @@
       <c r="T75" s="46"/>
     </row>
     <row r="76" spans="1:90" ht="22" customHeight="1">
-      <c r="A76" s="73"/>
-      <c r="B76" s="65"/>
-      <c r="C76" s="76"/>
-      <c r="D76" s="77"/>
-      <c r="E76" s="77"/>
-      <c r="F76" s="83"/>
-      <c r="G76" s="76"/>
-      <c r="H76" s="77"/>
-      <c r="I76" s="77"/>
-      <c r="J76" s="77"/>
+      <c r="A76" s="87"/>
+      <c r="B76" s="89"/>
+      <c r="C76" s="53"/>
+      <c r="D76" s="54"/>
+      <c r="E76" s="54"/>
+      <c r="F76" s="55"/>
+      <c r="G76" s="53"/>
+      <c r="H76" s="54"/>
+      <c r="I76" s="54"/>
+      <c r="J76" s="54"/>
       <c r="K76" s="40"/>
       <c r="L76" s="40"/>
       <c r="M76" s="40"/>
@@ -5526,16 +5574,16 @@
       <c r="T76" s="46"/>
     </row>
     <row r="77" spans="1:90" s="27" customFormat="1" ht="11">
-      <c r="A77" s="56"/>
-      <c r="B77" s="57"/>
-      <c r="C77" s="57"/>
-      <c r="D77" s="57"/>
-      <c r="E77" s="57"/>
-      <c r="F77" s="57"/>
-      <c r="G77" s="57"/>
-      <c r="H77" s="57"/>
-      <c r="I77" s="57"/>
-      <c r="J77" s="57"/>
+      <c r="A77" s="79"/>
+      <c r="B77" s="80"/>
+      <c r="C77" s="80"/>
+      <c r="D77" s="80"/>
+      <c r="E77" s="80"/>
+      <c r="F77" s="80"/>
+      <c r="G77" s="80"/>
+      <c r="H77" s="80"/>
+      <c r="I77" s="80"/>
+      <c r="J77" s="80"/>
       <c r="K77" s="42"/>
       <c r="L77" s="42"/>
       <c r="M77" s="42"/>
@@ -5590,9 +5638,9 @@
       <c r="B79" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C79" s="58"/>
-      <c r="D79" s="59"/>
-      <c r="E79" s="59"/>
+      <c r="C79" s="59"/>
+      <c r="D79" s="60"/>
+      <c r="E79" s="60"/>
       <c r="F79" s="3" t="s">
         <v>9</v>
       </c>
@@ -6225,11 +6273,11 @@
       <c r="CL85" s="37"/>
     </row>
     <row r="86" spans="1:90" ht="22">
-      <c r="A86" s="86" t="s">
+      <c r="A86" s="90" t="s">
         <v>23</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C86" s="12">
         <f>SUM(C80:C85)</f>
@@ -6246,12 +6294,12 @@
       <c r="F86" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G86" s="62" t="s">
+      <c r="G86" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="H86" s="63"/>
-      <c r="I86" s="63"/>
-      <c r="J86" s="63"/>
+      <c r="H86" s="64"/>
+      <c r="I86" s="64"/>
+      <c r="J86" s="64"/>
       <c r="K86" s="40"/>
       <c r="L86" s="40"/>
       <c r="M86" s="40"/>
@@ -6264,24 +6312,24 @@
       <c r="T86" s="46"/>
     </row>
     <row r="87" spans="1:90" ht="24">
-      <c r="A87" s="87"/>
+      <c r="A87" s="91"/>
       <c r="B87" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C87" s="93">
+        <v>25</v>
+      </c>
+      <c r="C87" s="56">
         <f>SUM(C86:E86)</f>
         <v>32.340000000000003</v>
       </c>
-      <c r="D87" s="94"/>
-      <c r="E87" s="94"/>
-      <c r="F87" s="95"/>
-      <c r="G87" s="91">
+      <c r="D87" s="57"/>
+      <c r="E87" s="57"/>
+      <c r="F87" s="58"/>
+      <c r="G87" s="65">
         <f>ROUNDUP(SUM(C86:E86)/3,2)</f>
         <v>10.78</v>
       </c>
-      <c r="H87" s="92"/>
-      <c r="I87" s="92"/>
-      <c r="J87" s="92"/>
+      <c r="H87" s="66"/>
+      <c r="I87" s="66"/>
+      <c r="J87" s="66"/>
       <c r="K87" s="40"/>
       <c r="L87" s="40"/>
       <c r="M87" s="40"/>
@@ -6294,22 +6342,22 @@
       <c r="T87" s="46"/>
     </row>
     <row r="88" spans="1:90" ht="22" customHeight="1">
-      <c r="A88" s="66"/>
+      <c r="A88" s="67"/>
       <c r="B88" s="24"/>
-      <c r="C88" s="50">
+      <c r="C88" s="73">
         <f>C87</f>
         <v>32.340000000000003</v>
       </c>
-      <c r="D88" s="51"/>
-      <c r="E88" s="51"/>
-      <c r="F88" s="52"/>
-      <c r="G88" s="68">
+      <c r="D88" s="74"/>
+      <c r="E88" s="74"/>
+      <c r="F88" s="75"/>
+      <c r="G88" s="69">
         <f>G87</f>
         <v>10.78</v>
       </c>
-      <c r="H88" s="69"/>
-      <c r="I88" s="69"/>
-      <c r="J88" s="69"/>
+      <c r="H88" s="70"/>
+      <c r="I88" s="70"/>
+      <c r="J88" s="70"/>
       <c r="K88" s="40"/>
       <c r="L88" s="40"/>
       <c r="M88" s="40"/>
@@ -6322,16 +6370,16 @@
       <c r="T88" s="46"/>
     </row>
     <row r="89" spans="1:90" ht="22" customHeight="1">
-      <c r="A89" s="67"/>
+      <c r="A89" s="68"/>
       <c r="B89" s="24"/>
-      <c r="C89" s="53"/>
-      <c r="D89" s="54"/>
-      <c r="E89" s="54"/>
-      <c r="F89" s="55"/>
-      <c r="G89" s="70"/>
-      <c r="H89" s="71"/>
-      <c r="I89" s="71"/>
-      <c r="J89" s="71"/>
+      <c r="C89" s="76"/>
+      <c r="D89" s="77"/>
+      <c r="E89" s="77"/>
+      <c r="F89" s="78"/>
+      <c r="G89" s="71"/>
+      <c r="H89" s="72"/>
+      <c r="I89" s="72"/>
+      <c r="J89" s="72"/>
       <c r="K89" s="40"/>
       <c r="L89" s="40"/>
       <c r="M89" s="40"/>
@@ -6344,16 +6392,16 @@
       <c r="T89" s="46"/>
     </row>
     <row r="90" spans="1:90" s="28" customFormat="1" ht="7">
-      <c r="A90" s="84"/>
-      <c r="B90" s="85"/>
-      <c r="C90" s="85"/>
-      <c r="D90" s="85"/>
-      <c r="E90" s="85"/>
-      <c r="F90" s="85"/>
-      <c r="G90" s="85"/>
-      <c r="H90" s="85"/>
-      <c r="I90" s="85"/>
-      <c r="J90" s="85"/>
+      <c r="A90" s="92"/>
+      <c r="B90" s="93"/>
+      <c r="C90" s="93"/>
+      <c r="D90" s="93"/>
+      <c r="E90" s="93"/>
+      <c r="F90" s="93"/>
+      <c r="G90" s="93"/>
+      <c r="H90" s="93"/>
+      <c r="I90" s="93"/>
+      <c r="J90" s="93"/>
       <c r="K90" s="43"/>
       <c r="L90" s="43"/>
       <c r="M90" s="43"/>
@@ -6408,9 +6456,9 @@
       <c r="B92" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C92" s="58"/>
-      <c r="D92" s="59"/>
-      <c r="E92" s="59"/>
+      <c r="C92" s="59"/>
+      <c r="D92" s="60"/>
+      <c r="E92" s="60"/>
       <c r="F92" s="3" t="s">
         <v>9</v>
       </c>
@@ -6928,11 +6976,11 @@
       <c r="BS98" s="37"/>
     </row>
     <row r="99" spans="1:71" ht="22">
-      <c r="A99" s="86" t="s">
+      <c r="A99" s="90" t="s">
         <v>24</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C99" s="17">
         <f>SUM(C93:C98)</f>
@@ -6947,12 +6995,12 @@
         <v>9.27</v>
       </c>
       <c r="F99" s="3"/>
-      <c r="G99" s="62" t="s">
+      <c r="G99" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="H99" s="63"/>
-      <c r="I99" s="63"/>
-      <c r="J99" s="63"/>
+      <c r="H99" s="64"/>
+      <c r="I99" s="64"/>
+      <c r="J99" s="64"/>
       <c r="K99" s="40"/>
       <c r="L99" s="40"/>
       <c r="M99" s="40"/>
@@ -6960,24 +7008,24 @@
       <c r="O99" s="40"/>
     </row>
     <row r="100" spans="1:71" ht="22">
-      <c r="A100" s="87"/>
+      <c r="A100" s="91"/>
       <c r="B100" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C100" s="88">
+        <v>25</v>
+      </c>
+      <c r="C100" s="83">
         <f>SUM(C99:E99)</f>
         <v>28.02</v>
       </c>
-      <c r="D100" s="89"/>
-      <c r="E100" s="89"/>
-      <c r="F100" s="90"/>
-      <c r="G100" s="62">
+      <c r="D100" s="84"/>
+      <c r="E100" s="84"/>
+      <c r="F100" s="85"/>
+      <c r="G100" s="63">
         <f>ROUNDUP(SUM(C99:E99)/3,2)</f>
         <v>9.34</v>
       </c>
-      <c r="H100" s="63"/>
-      <c r="I100" s="63"/>
-      <c r="J100" s="63"/>
+      <c r="H100" s="64"/>
+      <c r="I100" s="64"/>
+      <c r="J100" s="64"/>
       <c r="K100" s="40"/>
       <c r="L100" s="40"/>
       <c r="M100" s="40"/>
@@ -6985,24 +7033,24 @@
       <c r="O100" s="40"/>
     </row>
     <row r="101" spans="1:71" ht="22" customHeight="1">
-      <c r="A101" s="72"/>
-      <c r="B101" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="C101" s="74">
+      <c r="A101" s="86"/>
+      <c r="B101" s="88" t="s">
+        <v>27</v>
+      </c>
+      <c r="C101" s="50">
         <f>SUM(C88+C100)</f>
         <v>60.36</v>
       </c>
-      <c r="D101" s="75"/>
-      <c r="E101" s="75"/>
-      <c r="F101" s="82"/>
-      <c r="G101" s="74">
+      <c r="D101" s="51"/>
+      <c r="E101" s="51"/>
+      <c r="F101" s="52"/>
+      <c r="G101" s="50">
         <f>SUM(G88+G100)</f>
         <v>20.119999999999997</v>
       </c>
-      <c r="H101" s="75"/>
-      <c r="I101" s="75"/>
-      <c r="J101" s="75"/>
+      <c r="H101" s="51"/>
+      <c r="I101" s="51"/>
+      <c r="J101" s="51"/>
       <c r="K101" s="40"/>
       <c r="L101" s="40"/>
       <c r="M101" s="40"/>
@@ -7010,16 +7058,16 @@
       <c r="O101" s="40"/>
     </row>
     <row r="102" spans="1:71" ht="22" customHeight="1">
-      <c r="A102" s="73"/>
-      <c r="B102" s="65"/>
-      <c r="C102" s="76"/>
-      <c r="D102" s="77"/>
-      <c r="E102" s="77"/>
-      <c r="F102" s="83"/>
-      <c r="G102" s="76"/>
-      <c r="H102" s="77"/>
-      <c r="I102" s="77"/>
-      <c r="J102" s="77"/>
+      <c r="A102" s="87"/>
+      <c r="B102" s="89"/>
+      <c r="C102" s="53"/>
+      <c r="D102" s="54"/>
+      <c r="E102" s="54"/>
+      <c r="F102" s="55"/>
+      <c r="G102" s="53"/>
+      <c r="H102" s="54"/>
+      <c r="I102" s="54"/>
+      <c r="J102" s="54"/>
       <c r="K102" s="40"/>
       <c r="L102" s="40"/>
       <c r="M102" s="40"/>
@@ -7044,10 +7092,10 @@
       <c r="O103" s="40"/>
     </row>
     <row r="104" spans="1:71" s="35" customFormat="1" ht="32">
-      <c r="A104" s="78" t="s">
-        <v>29</v>
-      </c>
-      <c r="B104" s="79"/>
+      <c r="A104" s="94" t="s">
+        <v>28</v>
+      </c>
+      <c r="B104" s="95"/>
       <c r="C104" s="32">
         <f>SUM(C9+C22+C34+C47+C60+C73+C86+C99)</f>
         <v>110.46</v>
@@ -7060,13 +7108,15 @@
         <f>SUM(E9+E22+E34+E47+E60+E73+E86+E99)</f>
         <v>107.98000000000002</v>
       </c>
-      <c r="F104" s="80" t="s">
-        <v>25</v>
-      </c>
-      <c r="G104" s="81"/>
-      <c r="H104" s="81"/>
-      <c r="I104" s="81"/>
-      <c r="J104" s="81"/>
+      <c r="F104" s="96" t="s">
+        <v>46</v>
+      </c>
+      <c r="G104" s="96"/>
+      <c r="H104" s="96"/>
+      <c r="I104" s="97">
+        <v>63726</v>
+      </c>
+      <c r="J104" s="97"/>
       <c r="K104" s="44"/>
       <c r="L104" s="44"/>
       <c r="M104" s="44"/>
@@ -7074,67 +7124,7 @@
       <c r="O104" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="76">
-    <mergeCell ref="C24:F25"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="G11:J12"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F12"/>
-    <mergeCell ref="A38:J38"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="G47:J47"/>
-    <mergeCell ref="G48:J48"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="G49:J50"/>
-    <mergeCell ref="A51:J51"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="G60:J60"/>
-    <mergeCell ref="G61:J61"/>
-    <mergeCell ref="C49:F50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C61:F61"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="G62:J63"/>
-    <mergeCell ref="A64:J64"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="G73:J73"/>
-    <mergeCell ref="G74:J74"/>
-    <mergeCell ref="C74:F74"/>
-    <mergeCell ref="C62:F63"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="G75:J76"/>
-    <mergeCell ref="A77:J77"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="G86:J86"/>
-    <mergeCell ref="G87:J87"/>
-    <mergeCell ref="C87:F87"/>
-    <mergeCell ref="C75:F76"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="G88:J89"/>
-    <mergeCell ref="A90:J90"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="G99:J99"/>
-    <mergeCell ref="G100:J100"/>
-    <mergeCell ref="C100:F100"/>
-    <mergeCell ref="C88:F89"/>
-    <mergeCell ref="A101:A102"/>
-    <mergeCell ref="G101:J102"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="F104:J104"/>
-    <mergeCell ref="C101:F102"/>
-    <mergeCell ref="B101:B102"/>
+  <mergeCells count="77">
     <mergeCell ref="C36:F37"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="C15:E15"/>
@@ -7151,6 +7141,67 @@
     <mergeCell ref="G34:J34"/>
     <mergeCell ref="G35:J35"/>
     <mergeCell ref="C23:F23"/>
+    <mergeCell ref="A101:A102"/>
+    <mergeCell ref="G101:J102"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="C101:F102"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="G88:J89"/>
+    <mergeCell ref="A90:J90"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="G99:J99"/>
+    <mergeCell ref="G100:J100"/>
+    <mergeCell ref="C100:F100"/>
+    <mergeCell ref="C88:F89"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="G75:J76"/>
+    <mergeCell ref="A77:J77"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="G86:J86"/>
+    <mergeCell ref="G87:J87"/>
+    <mergeCell ref="C87:F87"/>
+    <mergeCell ref="C75:F76"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="G62:J63"/>
+    <mergeCell ref="A64:J64"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="G73:J73"/>
+    <mergeCell ref="G74:J74"/>
+    <mergeCell ref="C74:F74"/>
+    <mergeCell ref="C62:F63"/>
+    <mergeCell ref="G60:J60"/>
+    <mergeCell ref="G61:J61"/>
+    <mergeCell ref="C49:F50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C61:F61"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="G11:J12"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F12"/>
+    <mergeCell ref="C24:F25"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="I104:J104"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A38:J38"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="G47:J47"/>
+    <mergeCell ref="G48:J48"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="G49:J50"/>
+    <mergeCell ref="A51:J51"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="A60:A61"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -7179,7 +7230,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -7357,12 +7408,77 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A813D41-915D-4A49-8729-AF9A8D0544B2}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>